<commit_message>
superdataset-11 test with mae
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-2.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-11.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-12.csv)</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J57"/>
+  <dimension ref="C3:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,9 +394,11 @@
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -402,8 +407,12 @@
         <v>5</v>
       </c>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -418,8 +427,15 @@
       <c r="J4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -432,10 +448,19 @@
       <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="3">
+        <v>103.33917029511341</v>
+      </c>
+      <c r="J5" s="3">
+        <v>291.33735976789092</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -450,10 +475,20 @@
         <f>H5+1</f>
         <v>2</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="3">
+        <v>103.2342404450892</v>
+      </c>
+      <c r="J6" s="3">
+        <v>287.42223887814242</v>
+      </c>
+      <c r="M6" s="2">
+        <f>M5+1</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -468,10 +503,20 @@
         <f t="shared" ref="H7:H54" si="1">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="3">
+        <v>106.7087808417994</v>
+      </c>
+      <c r="J7" s="3">
+        <v>265.17763056092758</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:M54" si="2">M6+1</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -486,10 +531,20 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="3">
+        <v>103.4929874213833</v>
+      </c>
+      <c r="J8" s="3">
+        <v>275.21029013539572</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -504,10 +559,20 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="3">
+        <v>103.7085510401545</v>
+      </c>
+      <c r="J9" s="3">
+        <v>309.39573984526032</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -522,10 +587,20 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="3">
+        <v>107.968676826318</v>
+      </c>
+      <c r="J10" s="3">
+        <v>261.7416392649896</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -540,10 +615,20 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="3">
+        <v>103.6542597968067</v>
+      </c>
+      <c r="J11" s="3">
+        <v>285.63451644100508</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -558,10 +643,20 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="3">
+        <v>104.74070512820479</v>
+      </c>
+      <c r="J12" s="3">
+        <v>269.75672147001848</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -576,10 +671,20 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="3">
+        <v>104.42352564102529</v>
+      </c>
+      <c r="J13" s="3">
+        <v>287.13490328820041</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -594,10 +699,20 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="3">
+        <v>104.2551947266567</v>
+      </c>
+      <c r="J14" s="3">
+        <v>286.7637475822043</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -612,10 +727,20 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="3">
+        <v>105.62047169811289</v>
+      </c>
+      <c r="J15" s="3">
+        <v>271.01127659574388</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -630,10 +755,20 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="3">
+        <v>102.2240578132556</v>
+      </c>
+      <c r="J16" s="3">
+        <v>289.07830270792959</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -648,10 +783,20 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="3">
+        <v>105.73578616352169</v>
+      </c>
+      <c r="J17" s="3">
+        <v>272.8486266924557</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -666,10 +811,20 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="3">
+        <v>104.1674709724235</v>
+      </c>
+      <c r="J18" s="3">
+        <v>275.90771760154661</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -684,10 +839,20 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="3">
+        <v>106.66531325592619</v>
+      </c>
+      <c r="J19" s="3">
+        <v>257.29312379110172</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -702,10 +867,20 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="3">
+        <v>105.0770621673921</v>
+      </c>
+      <c r="J20" s="3">
+        <v>269.57683752417711</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -720,10 +895,20 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="3">
+        <v>103.9270149975807</v>
+      </c>
+      <c r="J21" s="3">
+        <v>271.11316247582118</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -738,10 +923,20 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="3">
+        <v>104.0905345911946</v>
+      </c>
+      <c r="J22" s="3">
+        <v>294.82047388781348</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -756,10 +951,20 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="3">
+        <v>101.69011490082219</v>
+      </c>
+      <c r="J23" s="3">
+        <v>294.57498065763929</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -774,10 +979,20 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="3">
+        <v>103.42047774552459</v>
+      </c>
+      <c r="J24" s="3">
+        <v>292.39652321083088</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -792,10 +1007,20 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="3">
+        <v>104.72240566037701</v>
+      </c>
+      <c r="J25" s="3">
+        <v>287.92470986460262</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -810,10 +1035,20 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="3">
+        <v>103.09516207063351</v>
+      </c>
+      <c r="J26" s="3">
+        <v>301.24157156673027</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -828,10 +1063,20 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="3">
+        <v>104.28720004837901</v>
+      </c>
+      <c r="J27" s="3">
+        <v>298.35047388781351</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -846,10 +1091,20 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I28" s="3">
+        <v>104.7571903725203</v>
+      </c>
+      <c r="J28" s="3">
+        <v>294.21959381044411</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -864,10 +1119,20 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I29" s="3">
+        <v>105.6352104499271</v>
+      </c>
+      <c r="J29" s="3">
+        <v>261.35097678916748</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -882,10 +1147,20 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I30" s="3">
+        <v>105.51058176100599</v>
+      </c>
+      <c r="J30" s="3">
+        <v>283.50336557059882</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -900,10 +1175,20 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I31" s="3">
+        <v>103.42625786163489</v>
+      </c>
+      <c r="J31" s="3">
+        <v>289.02388297872261</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -918,10 +1203,20 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I32" s="3">
+        <v>104.50952588292181</v>
+      </c>
+      <c r="J32" s="3">
+        <v>295.07449709864528</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -936,10 +1231,20 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="3">
+        <v>106.1680720851472</v>
+      </c>
+      <c r="J33" s="3">
+        <v>249.67743230174011</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -954,10 +1259,20 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="3">
+        <v>104.3139900822445</v>
+      </c>
+      <c r="J34" s="3">
+        <v>285.31301740812302</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -972,10 +1287,20 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="3">
+        <v>105.1388909046925</v>
+      </c>
+      <c r="J35" s="3">
+        <v>277.21365570599528</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -990,10 +1315,20 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="3">
+        <v>106.62778422835</v>
+      </c>
+      <c r="J36" s="3">
+        <v>256.41816247582119</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1008,10 +1343,20 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="3">
+        <v>104.4387868892111</v>
+      </c>
+      <c r="J37" s="3">
+        <v>278.68490812379031</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1026,10 +1371,20 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="3">
+        <v>104.25354862118979</v>
+      </c>
+      <c r="J38" s="3">
+        <v>287.62773694390631</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1044,10 +1399,20 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="3">
+        <v>101.7167803580065</v>
+      </c>
+      <c r="J39" s="3">
+        <v>303.71118471953503</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1062,10 +1427,20 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="3">
+        <v>102.3860546686015</v>
+      </c>
+      <c r="J40" s="3">
+        <v>290.70545938104368</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1080,10 +1455,20 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="3">
+        <v>107.0865493468792</v>
+      </c>
+      <c r="J41" s="3">
+        <v>261.62058027079217</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1098,10 +1483,20 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="3">
+        <v>106.11799104983039</v>
+      </c>
+      <c r="J42" s="3">
+        <v>271.37591392649819</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1116,10 +1511,20 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="3">
+        <v>102.9944279148521</v>
+      </c>
+      <c r="J43" s="3">
+        <v>277.05515957446721</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1134,10 +1539,20 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I44" s="3">
+        <v>104.66886913401029</v>
+      </c>
+      <c r="J44" s="3">
+        <v>276.35144100580192</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1152,10 +1567,20 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I45" s="3">
+        <v>101.31500120948201</v>
+      </c>
+      <c r="J45" s="3">
+        <v>296.04885396518301</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1170,10 +1595,20 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I46" s="3">
+        <v>106.5219533139813</v>
+      </c>
+      <c r="J46" s="3">
+        <v>262.57159090909011</v>
+      </c>
+      <c r="M46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1188,10 +1623,20 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I47" s="3">
+        <v>105.54287856797259</v>
+      </c>
+      <c r="J47" s="3">
+        <v>271.6435589941965</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1206,10 +1651,20 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I48" s="3">
+        <v>105.6280079825832</v>
+      </c>
+      <c r="J48" s="3">
+        <v>288.11954545454472</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1224,10 +1679,20 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="3">
+        <v>107.2841557813253</v>
+      </c>
+      <c r="J49" s="3">
+        <v>245.61797872340341</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1242,10 +1707,20 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="3">
+        <v>104.4679970972421</v>
+      </c>
+      <c r="J50" s="3">
+        <v>275.15124274661429</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1260,10 +1735,20 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="3">
+        <v>105.63250846637609</v>
+      </c>
+      <c r="J51" s="3">
+        <v>261.73852514506689</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1278,10 +1763,20 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="3">
+        <v>104.0001378809866</v>
+      </c>
+      <c r="J52" s="3">
+        <v>290.62776112185611</v>
+      </c>
+      <c r="M52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1296,10 +1791,20 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="3">
+        <v>102.9421020803093</v>
+      </c>
+      <c r="J53" s="3">
+        <v>296.29265957446728</v>
+      </c>
+      <c r="M53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1314,10 +1819,20 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I54" s="3">
+        <v>105.19136429608101</v>
+      </c>
+      <c r="J54" s="3">
+        <v>263.76137814313262</v>
+      </c>
+      <c r="M54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1332,16 +1847,27 @@
       <c r="H56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I56" s="3" t="e">
+      <c r="I56" s="3">
         <f>AVERAGE(I5:I54)</f>
+        <v>104.57051565070117</v>
+      </c>
+      <c r="J56" s="3">
+        <f>AVERAGE(J5:J54)</f>
+        <v>279.72425261121776</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N56" s="3" t="e">
+        <f>AVERAGE(N5:N54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J56" s="3" t="e">
-        <f>AVERAGE(J5:J54)</f>
+      <c r="O56" s="3" t="e">
+        <f>AVERAGE(O5:O54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1356,12 +1882,23 @@
       <c r="H57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="3" t="e">
+      <c r="I57" s="3">
         <f>_xlfn.STDEV.S(I5:I54)</f>
+        <v>1.503452378742818</v>
+      </c>
+      <c r="J57" s="3">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>14.746671677618719</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N57" s="3" t="e">
+        <f>_xlfn.STDEV.S(N5:N54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J57" s="3" t="e">
-        <f>_xlfn.STDEV.S(J5:J54)</f>
+      <c r="O57" s="3" t="e">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset-12 test with mae
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-2.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-12.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-13.csv)</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:O57"/>
+  <dimension ref="C3:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,9 +399,11 @@
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -411,8 +416,12 @@
         <v>6</v>
       </c>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -434,8 +443,15 @@
       <c r="O4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -457,10 +473,19 @@
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N5" s="3">
+        <v>107.3767948717945</v>
+      </c>
+      <c r="O5" s="3">
+        <v>263.16823500967041</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -485,10 +510,20 @@
         <f>M5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="3">
+        <v>103.9961901306238</v>
+      </c>
+      <c r="O6" s="3">
+        <v>308.98518375241702</v>
+      </c>
+      <c r="R6" s="2">
+        <f>R5+1</f>
+        <v>2</v>
+      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -513,10 +548,20 @@
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="3">
+        <v>105.21026487663249</v>
+      </c>
+      <c r="O7" s="3">
+        <v>273.41595744680768</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" ref="R7:R54" si="3">R6+1</f>
+        <v>3</v>
+      </c>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -541,10 +586,20 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="3">
+        <v>105.82911223996101</v>
+      </c>
+      <c r="O8" s="3">
+        <v>287.33444874274579</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -569,10 +624,20 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="3">
+        <v>106.37773826802101</v>
+      </c>
+      <c r="O9" s="3">
+        <v>276.67321083172072</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -597,10 +662,20 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="3">
+        <v>110.1779946782774</v>
+      </c>
+      <c r="O10" s="3">
+        <v>232.34365087040541</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -625,10 +700,20 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N11" s="3">
+        <v>106.2021432027089</v>
+      </c>
+      <c r="O11" s="3">
+        <v>265.95573984526033</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -653,10 +738,20 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N12" s="3">
+        <v>107.2859458151908</v>
+      </c>
+      <c r="O12" s="3">
+        <v>294.55427466150792</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -681,10 +776,20 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="3">
+        <v>104.49681785195909</v>
+      </c>
+      <c r="O13" s="3">
+        <v>286.11062862669172</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -709,10 +814,20 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="3">
+        <v>106.90281930333779</v>
+      </c>
+      <c r="O14" s="3">
+        <v>279.83248549322929</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -737,10 +852,20 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="3">
+        <v>104.26868408321209</v>
+      </c>
+      <c r="O15" s="3">
+        <v>282.84857350096632</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -765,10 +890,20 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N16" s="3">
+        <v>103.6387360909528</v>
+      </c>
+      <c r="O16" s="3">
+        <v>287.30325435203008</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -793,10 +928,20 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="3">
+        <v>103.2830587808415</v>
+      </c>
+      <c r="O17" s="3">
+        <v>317.92928916827771</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -821,10 +966,20 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N18" s="3">
+        <v>106.7507728592159</v>
+      </c>
+      <c r="O18" s="3">
+        <v>283.92850096711709</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -849,10 +1004,20 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N19" s="3">
+        <v>101.8109579100142</v>
+      </c>
+      <c r="O19" s="3">
+        <v>315.27785783365482</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -877,10 +1042,20 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N20" s="3">
+        <v>103.98487663280081</v>
+      </c>
+      <c r="O20" s="3">
+        <v>277.03888781431249</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -905,10 +1080,20 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="3">
+        <v>106.3650326560229</v>
+      </c>
+      <c r="O21" s="3">
+        <v>263.51261121856788</v>
+      </c>
+      <c r="R21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -933,10 +1118,20 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N22" s="3">
+        <v>105.9923234155778</v>
+      </c>
+      <c r="O22" s="3">
+        <v>289.46270309477683</v>
+      </c>
+      <c r="R22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -961,10 +1156,20 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="3">
+        <v>104.73290154813709</v>
+      </c>
+      <c r="O23" s="3">
+        <v>298.42606866537642</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -989,10 +1194,20 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N24" s="3">
+        <v>103.25519109820971</v>
+      </c>
+      <c r="O24" s="3">
+        <v>297.66118955512491</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1017,10 +1232,20 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N25" s="3">
+        <v>104.8970077406867</v>
+      </c>
+      <c r="O25" s="3">
+        <v>282.33883945841308</v>
+      </c>
+      <c r="R25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1045,10 +1270,20 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N26" s="3">
+        <v>103.7638304305754</v>
+      </c>
+      <c r="O26" s="3">
+        <v>283.67149903288117</v>
+      </c>
+      <c r="R26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1073,10 +1308,20 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N27" s="3">
+        <v>103.5331555394288</v>
+      </c>
+      <c r="O27" s="3">
+        <v>303.6760880077361</v>
+      </c>
+      <c r="R27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1101,10 +1346,20 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N28" s="3">
+        <v>107.9670222544748</v>
+      </c>
+      <c r="O28" s="3">
+        <v>272.28766441005718</v>
+      </c>
+      <c r="R28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1129,10 +1384,20 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N29" s="3">
+        <v>105.23941823899339</v>
+      </c>
+      <c r="O29" s="3">
+        <v>294.6469535783358</v>
+      </c>
+      <c r="R29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1157,10 +1422,20 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="3">
+        <v>108.18436018384099</v>
+      </c>
+      <c r="O30" s="3">
+        <v>272.6700435203087</v>
+      </c>
+      <c r="R30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1185,10 +1460,20 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N31" s="3">
+        <v>105.28175374939489</v>
+      </c>
+      <c r="O31" s="3">
+        <v>271.76751450676898</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1213,10 +1498,20 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N32" s="3">
+        <v>105.41104862118981</v>
+      </c>
+      <c r="O32" s="3">
+        <v>278.71871373307459</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1241,10 +1536,20 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N33" s="3">
+        <v>105.6928072085144</v>
+      </c>
+      <c r="O33" s="3">
+        <v>283.54942456479608</v>
+      </c>
+      <c r="R33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1269,10 +1574,20 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N34" s="3">
+        <v>106.1145597484274</v>
+      </c>
+      <c r="O34" s="3">
+        <v>290.24460348162393</v>
+      </c>
+      <c r="R34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1297,10 +1612,20 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N35" s="3">
+        <v>106.33048137397159</v>
+      </c>
+      <c r="O35" s="3">
+        <v>287.87925048355822</v>
+      </c>
+      <c r="R35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1325,10 +1650,20 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N36" s="3">
+        <v>106.9850302370582</v>
+      </c>
+      <c r="O36" s="3">
+        <v>276.30514023210759</v>
+      </c>
+      <c r="R36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1353,10 +1688,20 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-    </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N37" s="3">
+        <v>108.4757402031927</v>
+      </c>
+      <c r="O37" s="3">
+        <v>258.91448259187541</v>
+      </c>
+      <c r="R37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1381,10 +1726,20 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N38" s="3">
+        <v>103.9350689404932</v>
+      </c>
+      <c r="O38" s="3">
+        <v>303.42380560928348</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1409,10 +1764,20 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-    </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N39" s="3">
+        <v>106.80495766811769</v>
+      </c>
+      <c r="O39" s="3">
+        <v>268.0895261121849</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1437,10 +1802,20 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-    </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N40" s="3">
+        <v>105.04724963715501</v>
+      </c>
+      <c r="O40" s="3">
+        <v>294.79389748549238</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1465,10 +1840,20 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-    </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N41" s="3">
+        <v>105.8575677310108</v>
+      </c>
+      <c r="O41" s="3">
+        <v>280.15143133462198</v>
+      </c>
+      <c r="R41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1493,10 +1878,20 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-    </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N42" s="3">
+        <v>105.3744218674404</v>
+      </c>
+      <c r="O42" s="3">
+        <v>261.8615377176007</v>
+      </c>
+      <c r="R42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1521,10 +1916,20 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-    </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N43" s="3">
+        <v>105.2958684083209</v>
+      </c>
+      <c r="O43" s="3">
+        <v>286.54523694390639</v>
+      </c>
+      <c r="R43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1549,10 +1954,20 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-    </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N44" s="3">
+        <v>104.1758236574743</v>
+      </c>
+      <c r="O44" s="3">
+        <v>287.10972920696253</v>
+      </c>
+      <c r="R44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+    </row>
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1577,10 +1992,20 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-    </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N45" s="3">
+        <v>104.8145234639572</v>
+      </c>
+      <c r="O45" s="3">
+        <v>286.413592843326</v>
+      </c>
+      <c r="R45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+    </row>
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1605,10 +2030,20 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-    </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N46" s="3">
+        <v>105.1391944847602</v>
+      </c>
+      <c r="O46" s="3">
+        <v>274.93380077369358</v>
+      </c>
+      <c r="R46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+    </row>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1633,10 +2068,20 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-    </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N47" s="3">
+        <v>109.1802672955971</v>
+      </c>
+      <c r="O47" s="3">
+        <v>254.70756286266851</v>
+      </c>
+      <c r="R47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+    </row>
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1661,10 +2106,20 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-    </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N48" s="3">
+        <v>101.7788401064341</v>
+      </c>
+      <c r="O48" s="3">
+        <v>343.70193907156602</v>
+      </c>
+      <c r="R48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+    </row>
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1689,10 +2144,20 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-    </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N49" s="3">
+        <v>107.0740517658439</v>
+      </c>
+      <c r="O49" s="3">
+        <v>290.15515473887729</v>
+      </c>
+      <c r="R49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1717,10 +2182,20 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-    </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N50" s="3">
+        <v>108.9617283502658</v>
+      </c>
+      <c r="O50" s="3">
+        <v>260.31964700193339</v>
+      </c>
+      <c r="R50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+    </row>
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1745,10 +2220,20 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-    </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N51" s="3">
+        <v>106.4962481857762</v>
+      </c>
+      <c r="O51" s="3">
+        <v>270.87915860734921</v>
+      </c>
+      <c r="R51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+    </row>
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1773,10 +2258,20 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-    </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N52" s="3">
+        <v>106.88102685050769</v>
+      </c>
+      <c r="O52" s="3">
+        <v>279.4191537717594</v>
+      </c>
+      <c r="R52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+    </row>
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1801,10 +2296,20 @@
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-    </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N53" s="3">
+        <v>107.5499951620703</v>
+      </c>
+      <c r="O53" s="3">
+        <v>284.27007736943818</v>
+      </c>
+      <c r="R53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+    </row>
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1829,10 +2334,20 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="N54" s="3">
+        <v>106.1368335752295</v>
+      </c>
+      <c r="O54" s="3">
+        <v>278.31162959380958</v>
+      </c>
+      <c r="R54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+    </row>
+    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1858,16 +2373,27 @@
       <c r="M56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N56" s="3" t="e">
+      <c r="N56" s="3">
         <f>AVERAGE(N5:N54)</f>
+        <v>105.7263647798739</v>
+      </c>
+      <c r="O56" s="3">
+        <f>AVERAGE(O5:O54)</f>
+        <v>282.87039700193344</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S56" s="3" t="e">
+        <f>AVERAGE(S5:S54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O56" s="3" t="e">
-        <f>AVERAGE(O5:O54)</f>
+      <c r="T56" s="3" t="e">
+        <f>AVERAGE(T5:T54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1893,12 +2419,23 @@
       <c r="M57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N57" s="3" t="e">
+      <c r="N57" s="3">
         <f>_xlfn.STDEV.S(N5:N54)</f>
+        <v>1.7830857541936536</v>
+      </c>
+      <c r="O57" s="3">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>17.856998581266218</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S57" s="3" t="e">
+        <f>_xlfn.STDEV.S(S5:S54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O57" s="3" t="e">
-        <f>_xlfn.STDEV.S(O5:O54)</f>
+      <c r="T57" s="3" t="e">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset 13 (mae) & 10 (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-2.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-2.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAE" sheetId="1" r:id="rId1"/>
+    <sheet name="MSE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -43,6 +44,12 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-13.csv)</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
   </si>
 </sst>
 </file>
@@ -96,13 +103,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -387,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,8 +492,12 @@
       <c r="R5" s="2">
         <v>1</v>
       </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
+      <c r="S5" s="3">
+        <v>103.73361514271861</v>
+      </c>
+      <c r="T5" s="3">
+        <v>274.65105899419649</v>
+      </c>
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
@@ -520,8 +534,12 @@
         <f>R5+1</f>
         <v>2</v>
       </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
+      <c r="S6" s="3">
+        <v>99.480510401547832</v>
+      </c>
+      <c r="T6" s="3">
+        <v>300.48460831721388</v>
+      </c>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -558,8 +576,12 @@
         <f t="shared" ref="R7:R54" si="3">R6+1</f>
         <v>3</v>
       </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
+      <c r="S7" s="3">
+        <v>100.2885909530718</v>
+      </c>
+      <c r="T7" s="3">
+        <v>297.76296905222358</v>
+      </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -596,8 +618,12 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="S8" s="3">
+        <v>103.6732051282048</v>
+      </c>
+      <c r="T8" s="3">
+        <v>273.04195841392573</v>
+      </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -634,8 +660,12 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
+      <c r="S9" s="3">
+        <v>103.1198633284951</v>
+      </c>
+      <c r="T9" s="3">
+        <v>257.82382978723319</v>
+      </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -672,8 +702,12 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
+      <c r="S10" s="3">
+        <v>100.74140179003361</v>
+      </c>
+      <c r="T10" s="3">
+        <v>287.40967601547311</v>
+      </c>
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -710,8 +744,12 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
+      <c r="S11" s="3">
+        <v>102.6672363328492</v>
+      </c>
+      <c r="T11" s="3">
+        <v>258.10086073500901</v>
+      </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -748,8 +786,12 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="S12" s="3">
+        <v>100.4471915820026</v>
+      </c>
+      <c r="T12" s="3">
+        <v>291.49372340425452</v>
+      </c>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -786,8 +828,12 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
+      <c r="S13" s="3">
+        <v>104.65033865505529</v>
+      </c>
+      <c r="T13" s="3">
+        <v>270.54553191489282</v>
+      </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -824,8 +870,12 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
+      <c r="S14" s="3">
+        <v>101.68859337203649</v>
+      </c>
+      <c r="T14" s="3">
+        <v>261.10185686653688</v>
+      </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -862,8 +912,12 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
+      <c r="S15" s="3">
+        <v>102.6869968553456</v>
+      </c>
+      <c r="T15" s="3">
+        <v>262.31161025144991</v>
+      </c>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -900,8 +954,12 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
+      <c r="S16" s="3">
+        <v>100.1198584905657</v>
+      </c>
+      <c r="T16" s="3">
+        <v>297.60948259187529</v>
+      </c>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -938,8 +996,12 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
+      <c r="S17" s="3">
+        <v>102.86914247701959</v>
+      </c>
+      <c r="T17" s="3">
+        <v>274.84925048355819</v>
+      </c>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -976,8 +1038,12 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
+      <c r="S18" s="3">
+        <v>102.8740578132556</v>
+      </c>
+      <c r="T18" s="3">
+        <v>280.11029013539581</v>
+      </c>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -1014,8 +1080,12 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
+      <c r="S19" s="3">
+        <v>103.5737469762938</v>
+      </c>
+      <c r="T19" s="3">
+        <v>252.58670212765881</v>
+      </c>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -1052,8 +1122,12 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
+      <c r="S20" s="3">
+        <v>102.0787699564583</v>
+      </c>
+      <c r="T20" s="3">
+        <v>277.7396663442932</v>
+      </c>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -1090,8 +1164,12 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
+      <c r="S21" s="3">
+        <v>103.7656966618284</v>
+      </c>
+      <c r="T21" s="3">
+        <v>271.45968085106301</v>
+      </c>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -1128,8 +1206,12 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
+      <c r="S22" s="3">
+        <v>100.9580273343006</v>
+      </c>
+      <c r="T22" s="3">
+        <v>280.84002417794892</v>
+      </c>
     </row>
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -1166,8 +1248,12 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
+      <c r="S23" s="3">
+        <v>101.4577479438797</v>
+      </c>
+      <c r="T23" s="3">
+        <v>293.74333655705908</v>
+      </c>
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -1204,8 +1290,12 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
+      <c r="S24" s="3">
+        <v>102.4662445573292</v>
+      </c>
+      <c r="T24" s="3">
+        <v>282.72618955512479</v>
+      </c>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -1242,8 +1332,12 @@
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
+      <c r="S25" s="3">
+        <v>104.5536550556359</v>
+      </c>
+      <c r="T25" s="3">
+        <v>257.92569632495082</v>
+      </c>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -1280,8 +1374,12 @@
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
+      <c r="S26" s="3">
+        <v>102.9641872278662</v>
+      </c>
+      <c r="T26" s="3">
+        <v>273.79771760154659</v>
+      </c>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -1318,8 +1416,12 @@
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
+      <c r="S27" s="3">
+        <v>102.8248379293659</v>
+      </c>
+      <c r="T27" s="3">
+        <v>257.77653288201083</v>
+      </c>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -1356,8 +1458,12 @@
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
+      <c r="S28" s="3">
+        <v>99.500304789549773</v>
+      </c>
+      <c r="T28" s="3">
+        <v>284.24172630560838</v>
+      </c>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
@@ -1394,8 +1500,12 @@
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
+      <c r="S29" s="3">
+        <v>102.8506894049344</v>
+      </c>
+      <c r="T29" s="3">
+        <v>265.30017408123717</v>
+      </c>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
@@ -1432,8 +1542,12 @@
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
+      <c r="S30" s="3">
+        <v>103.58974358974331</v>
+      </c>
+      <c r="T30" s="3">
+        <v>277.44027562862601</v>
+      </c>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
@@ -1470,8 +1584,12 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
+      <c r="S31" s="3">
+        <v>102.25826681180421</v>
+      </c>
+      <c r="T31" s="3">
+        <v>281.64653771760072</v>
+      </c>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
@@ -1508,8 +1626,12 @@
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
+      <c r="S32" s="3">
+        <v>103.3072302854375</v>
+      </c>
+      <c r="T32" s="3">
+        <v>268.56069148936092</v>
+      </c>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
@@ -1546,8 +1668,12 @@
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
+      <c r="S33" s="3">
+        <v>102.00744920174139</v>
+      </c>
+      <c r="T33" s="3">
+        <v>293.82440038684638</v>
+      </c>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
@@ -1584,8 +1710,12 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
+      <c r="S34" s="3">
+        <v>102.428726415094</v>
+      </c>
+      <c r="T34" s="3">
+        <v>262.06911025145001</v>
+      </c>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
@@ -1622,8 +1752,12 @@
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
+      <c r="S35" s="3">
+        <v>103.8801838413156</v>
+      </c>
+      <c r="T35" s="3">
+        <v>277.19192456479612</v>
+      </c>
     </row>
     <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
@@ -1660,8 +1794,12 @@
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
+      <c r="S36" s="3">
+        <v>102.4217126269954</v>
+      </c>
+      <c r="T36" s="3">
+        <v>267.77281914893541</v>
+      </c>
     </row>
     <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
@@ -1698,8 +1836,12 @@
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
+      <c r="S37" s="3">
+        <v>100.4513957426219</v>
+      </c>
+      <c r="T37" s="3">
+        <v>282.78385880077292</v>
+      </c>
     </row>
     <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
@@ -1736,8 +1878,12 @@
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
+      <c r="S38" s="3">
+        <v>102.3767295597481</v>
+      </c>
+      <c r="T38" s="3">
+        <v>258.77467601547312</v>
+      </c>
     </row>
     <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
@@ -1774,8 +1920,12 @@
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
+      <c r="S39" s="3">
+        <v>102.5828531688434</v>
+      </c>
+      <c r="T39" s="3">
+        <v>274.68762572533763</v>
+      </c>
     </row>
     <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
@@ -1812,8 +1962,12 @@
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
+      <c r="S40" s="3">
+        <v>102.1518214804061</v>
+      </c>
+      <c r="T40" s="3">
+        <v>267.41830270792963</v>
+      </c>
     </row>
     <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
@@ -1850,8 +2004,12 @@
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
+      <c r="S41" s="3">
+        <v>99.758828011610717</v>
+      </c>
+      <c r="T41" s="3">
+        <v>298.6525483558986</v>
+      </c>
     </row>
     <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
@@ -1888,8 +2046,12 @@
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
+      <c r="S42" s="3">
+        <v>104.0349891146586</v>
+      </c>
+      <c r="T42" s="3">
+        <v>263.5406673114112</v>
+      </c>
     </row>
     <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
@@ -1926,8 +2088,12 @@
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
+      <c r="S43" s="3">
+        <v>103.9530902273824</v>
+      </c>
+      <c r="T43" s="3">
+        <v>268.06646034816168</v>
+      </c>
     </row>
     <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
@@ -1964,8 +2130,12 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
+      <c r="S44" s="3">
+        <v>101.65479801644869</v>
+      </c>
+      <c r="T44" s="3">
+        <v>273.42770309477669</v>
+      </c>
     </row>
     <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
@@ -2002,8 +2172,12 @@
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
+      <c r="S45" s="3">
+        <v>101.64799588775971</v>
+      </c>
+      <c r="T45" s="3">
+        <v>279.27834139264922</v>
+      </c>
     </row>
     <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
@@ -2040,8 +2214,12 @@
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
+      <c r="S46" s="3">
+        <v>103.93513062409259</v>
+      </c>
+      <c r="T46" s="3">
+        <v>278.94244680850989</v>
+      </c>
     </row>
     <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
@@ -2078,8 +2256,12 @@
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
+      <c r="S47" s="3">
+        <v>101.10636308659861</v>
+      </c>
+      <c r="T47" s="3">
+        <v>270.91570116054078</v>
+      </c>
     </row>
     <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
@@ -2116,8 +2298,12 @@
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
+      <c r="S48" s="3">
+        <v>102.6366279632314</v>
+      </c>
+      <c r="T48" s="3">
+        <v>272.83668278529899</v>
+      </c>
     </row>
     <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
@@ -2154,8 +2340,12 @@
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
+      <c r="S49" s="3">
+        <v>102.01430696661799</v>
+      </c>
+      <c r="T49" s="3">
+        <v>282.99298839458328</v>
+      </c>
     </row>
     <row r="50" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
@@ -2192,8 +2382,12 @@
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
+      <c r="S50" s="3">
+        <v>101.6041061925493</v>
+      </c>
+      <c r="T50" s="3">
+        <v>258.98455512572451</v>
+      </c>
     </row>
     <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
@@ -2230,8 +2424,12 @@
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
+      <c r="S51" s="3">
+        <v>103.2028531688434</v>
+      </c>
+      <c r="T51" s="3">
+        <v>272.8359574468077</v>
+      </c>
     </row>
     <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
@@ -2268,8 +2466,12 @@
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
+      <c r="S52" s="3">
+        <v>103.5947677793901</v>
+      </c>
+      <c r="T52" s="3">
+        <v>285.45289651837442</v>
+      </c>
     </row>
     <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
@@ -2306,8 +2508,12 @@
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="S53" s="3"/>
-      <c r="T53" s="3"/>
+      <c r="S53" s="3">
+        <v>103.3708006773098</v>
+      </c>
+      <c r="T53" s="3">
+        <v>259.88518858800688</v>
+      </c>
     </row>
     <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
@@ -2344,8 +2550,12 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="S54" s="3"/>
-      <c r="T54" s="3"/>
+      <c r="S54" s="3">
+        <v>103.92492864054159</v>
+      </c>
+      <c r="T54" s="3">
+        <v>254.84565280464139</v>
+      </c>
     </row>
     <row r="56" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
@@ -2384,13 +2594,13 @@
       <c r="R56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S56" s="3" t="e">
+      <c r="S56" s="3">
         <f>AVERAGE(S5:S54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T56" s="3" t="e">
+        <v>102.39860418480858</v>
+      </c>
+      <c r="T56" s="3">
         <f>AVERAGE(T5:T54)</f>
-        <v>#DIV/0!</v>
+        <v>274.36524332688504</v>
       </c>
     </row>
     <row r="57" spans="3:20" x14ac:dyDescent="0.25">
@@ -2430,12 +2640,1005 @@
       <c r="R57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="S57" s="3" t="e">
+      <c r="S57" s="3">
         <f>_xlfn.STDEV.S(S5:S54)</f>
+        <v>1.3308349991842039</v>
+      </c>
+      <c r="T57" s="3">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
+        <v>12.554493545564942</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:K57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5.8845023912725637E-5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4.4079670110362532E-4</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f>D5+1</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.7579371467027072E-5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4.9269773755610403E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <f>I5+1</f>
+        <v>2</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f t="shared" ref="D7:D54" si="0">D6+1</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5.3114235348158571E-5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>9.3532799093717922E-4</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I54" si="1">I6+1</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.5864878567241269E-5</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5.7325271579714921E-4</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6.189026273348386E-5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4.448844229250622E-4</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5.4022178298713493E-5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6.3372776975037471E-4</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E11" s="4">
+        <v>7.3474317815113577E-5</v>
+      </c>
+      <c r="F11" s="4">
+        <v>3.1313053740720978E-4</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="4">
+        <v>6.3423479791667394E-5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5.5026130243235642E-4</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5.8488751815980232E-5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>5.9591794408428629E-4</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6.4197694852781279E-5</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3.8800839261511611E-4</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E15" s="4">
+        <v>6.0739441251622618E-5</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4.0729317899633873E-4</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E16" s="4">
+        <v>7.2676622567253589E-5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5.5076989734064645E-4</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E17" s="4">
+        <v>6.9241403761771708E-5</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3.4388241446744891E-4</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E18" s="4">
+        <v>6.1101830791254066E-5</v>
+      </c>
+      <c r="F18" s="4">
+        <v>4.4004379524727351E-4</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E19" s="4">
+        <v>6.4706567010577637E-5</v>
+      </c>
+      <c r="F19" s="4">
+        <v>4.1791620955440898E-4</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E20" s="4">
+        <v>5.7237620750453773E-5</v>
+      </c>
+      <c r="F20" s="4">
+        <v>5.3876853363744555E-4</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E21" s="4">
+        <v>7.401270124286233E-5</v>
+      </c>
+      <c r="F21" s="4">
+        <v>2.5619509542017358E-4</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E22" s="4">
+        <v>7.2598111090185443E-5</v>
+      </c>
+      <c r="F22" s="4">
+        <v>4.4165939708170379E-4</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E23" s="4">
+        <v>7.2296474985281386E-5</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4.1773167914634871E-4</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E24" s="4">
+        <v>7.2188453166563689E-5</v>
+      </c>
+      <c r="F24" s="4">
+        <v>3.673350251113925E-4</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E25" s="4">
+        <v>6.2408880369377079E-5</v>
+      </c>
+      <c r="F25" s="4">
+        <v>3.0857245172557682E-4</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E26" s="4">
+        <v>7.0319306758594955E-5</v>
+      </c>
+      <c r="F26" s="4">
+        <v>4.1555415065531082E-4</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E27" s="4">
+        <v>6.3081717603864136E-5</v>
+      </c>
+      <c r="F27" s="4">
+        <v>4.4057954454082809E-4</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E28" s="4">
+        <v>7.3802346132725464E-5</v>
+      </c>
+      <c r="F28" s="4">
+        <v>4.6436490847260231E-4</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E29" s="4">
+        <v>6.4245717136023964E-5</v>
+      </c>
+      <c r="F29" s="4">
+        <v>3.5105760079538761E-4</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E30" s="4">
+        <v>7.0426780288361396E-5</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3.7928499391421251E-4</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E31" s="4">
+        <v>5.3070088116143212E-5</v>
+      </c>
+      <c r="F31" s="4">
+        <v>6.8801275653463171E-4</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E32" s="4">
+        <v>6.2679598314705601E-5</v>
+      </c>
+      <c r="F32" s="4">
+        <v>4.2101645522853908E-4</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E33" s="4">
+        <v>6.3070456599174246E-5</v>
+      </c>
+      <c r="F33" s="4">
+        <v>3.3849509164299779E-4</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E34" s="4">
+        <v>7.3104391430334919E-5</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3.3796426101693171E-4</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E35" s="4">
+        <v>6.9771644672017368E-5</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3.2881541412420031E-4</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E36" s="4">
+        <v>5.8294218018904167E-5</v>
+      </c>
+      <c r="F36" s="4">
+        <v>6.5361540120384561E-4</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E37" s="4">
+        <v>6.6731999163753208E-5</v>
+      </c>
+      <c r="F37" s="4">
+        <v>3.3951320703069212E-4</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E38" s="4">
+        <v>6.3353418231687213E-5</v>
+      </c>
+      <c r="F38" s="4">
+        <v>4.9734508277321878E-4</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E39" s="4">
+        <v>6.9695853919632503E-5</v>
+      </c>
+      <c r="F39" s="4">
+        <v>3.5520407492477642E-4</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E40" s="4">
+        <v>6.593546982349887E-5</v>
+      </c>
+      <c r="F40" s="4">
+        <v>4.5414907466677319E-4</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E41" s="4">
+        <v>6.3454149413689557E-5</v>
+      </c>
+      <c r="F41" s="4">
+        <v>4.6039503873827371E-4</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E42" s="4">
+        <v>5.5524637339811873E-5</v>
+      </c>
+      <c r="F42" s="4">
+        <v>7.1391621406034214E-4</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E43" s="4">
+        <v>6.4611071716630229E-5</v>
+      </c>
+      <c r="F43" s="4">
+        <v>3.9489282500487262E-4</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E44" s="4">
+        <v>5.6530989818356953E-5</v>
+      </c>
+      <c r="F44" s="4">
+        <v>5.4913444719626109E-4</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E45" s="4">
+        <v>6.0098690093020278E-5</v>
+      </c>
+      <c r="F45" s="4">
+        <v>6.4589302030280461E-4</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E46" s="4">
+        <v>6.7622086460276558E-5</v>
+      </c>
+      <c r="F46" s="4">
+        <v>2.7996775275789578E-4</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E47" s="4">
+        <v>6.9399552834462484E-5</v>
+      </c>
+      <c r="F47" s="4">
+        <v>4.2991660037973662E-4</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E48" s="4">
+        <v>6.1678967984429918E-5</v>
+      </c>
+      <c r="F48" s="4">
+        <v>4.7820022742944059E-4</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E49" s="4">
+        <v>5.7800767791620161E-5</v>
+      </c>
+      <c r="F49" s="4">
+        <v>6.0201595197629544E-4</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E50" s="4">
+        <v>7.0680487646653859E-5</v>
+      </c>
+      <c r="F50" s="4">
+        <v>4.7933646518839688E-4</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E51" s="4">
+        <v>6.4836396219702868E-5</v>
+      </c>
+      <c r="F51" s="4">
+        <v>3.6137972467754171E-4</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E52" s="4">
+        <v>6.1886138932292384E-5</v>
+      </c>
+      <c r="F52" s="4">
+        <v>4.7963596829745471E-4</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E53" s="4">
+        <v>6.5891542597639328E-5</v>
+      </c>
+      <c r="F53" s="4">
+        <v>2.4065946612863019E-4</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E54" s="4">
+        <v>6.4772236040643583E-5</v>
+      </c>
+      <c r="F54" s="4">
+        <v>4.9407298909470124E-4</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" s="4">
+        <f>AVERAGE(E5:E54)</f>
+        <v>6.4249580453774931E-5</v>
+      </c>
+      <c r="F56" s="4">
+        <f>AVERAGE(F5:F54)</f>
+        <v>4.5865123802189654E-4</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="4" t="e">
+        <f>AVERAGE(J5:J54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T57" s="3" t="e">
-        <f>_xlfn.STDEV.S(T5:T54)</f>
+      <c r="K56" s="4" t="e">
+        <f>AVERAGE(K5:K54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="4">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>5.9439383671645725E-6</v>
+      </c>
+      <c r="F57" s="4">
+        <f>_xlfn.STDEV.S(F5:F54)</f>
+        <v>1.3110803945559524E-4</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J57" s="4" t="e">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K57" s="4" t="e">
+        <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset 11 test with mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-2.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -2656,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:K57"/>
+  <dimension ref="D3:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,9 +2668,11 @@
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2679,8 +2681,12 @@
         <v>5</v>
       </c>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -2695,8 +2701,15 @@
       <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -2709,10 +2722,19 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="4">
+        <v>7.0874200231351315E-5</v>
+      </c>
+      <c r="K5" s="4">
+        <v>3.490213426590818E-4</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
@@ -2727,10 +2749,20 @@
         <f>I5+1</f>
         <v>2</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="4">
+        <v>6.08228496746671E-5</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3.5510666884648883E-4</v>
+      </c>
+      <c r="M6" s="2">
+        <f>M5+1</f>
+        <v>2</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
@@ -2745,10 +2777,20 @@
         <f t="shared" ref="I7:I54" si="1">I6+1</f>
         <v>3</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="4">
+        <v>7.4588663772628575E-5</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4.0006883167582788E-4</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:M54" si="2">M6+1</f>
+        <v>3</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2763,10 +2805,20 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="4">
+        <v>6.760046075251362E-5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2.9238078911649759E-4</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2781,10 +2833,20 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="4">
+        <v>6.8633019270915841E-5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>3.9455950933599818E-4</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2799,10 +2861,20 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="4">
+        <v>6.6988159880599052E-5</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.6907721090905107E-4</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2817,10 +2889,20 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="4">
+        <v>6.4653252323796127E-5</v>
+      </c>
+      <c r="K11" s="4">
+        <v>9.6792392962882865E-4</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2835,10 +2917,20 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="4">
+        <v>6.6273225706452559E-5</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2.8248852689565093E-4</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2853,10 +2945,20 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="4">
+        <v>6.7172450574515673E-5</v>
+      </c>
+      <c r="K13" s="4">
+        <v>3.5445521812474249E-4</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2871,10 +2973,20 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="4">
+        <v>6.7089918896920056E-5</v>
+      </c>
+      <c r="K14" s="4">
+        <v>4.4786002296544531E-4</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2889,10 +3001,20 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="4">
+        <v>6.5712575381257068E-5</v>
+      </c>
+      <c r="K15" s="4">
+        <v>4.0671076009897981E-4</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2907,10 +3029,20 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="4">
+        <v>5.4382150437259108E-5</v>
+      </c>
+      <c r="K16" s="4">
+        <v>6.5965253084427386E-4</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2925,10 +3057,20 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="4">
+        <v>5.5847883628644771E-5</v>
+      </c>
+      <c r="K17" s="4">
+        <v>6.6381434295174609E-4</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2943,10 +3085,20 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="4">
+        <v>6.5348132055882788E-5</v>
+      </c>
+      <c r="K18" s="4">
+        <v>3.8840750102423779E-4</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2961,10 +3113,20 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="4">
+        <v>6.702346638093486E-5</v>
+      </c>
+      <c r="K19" s="4">
+        <v>4.1043540166760571E-4</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2979,10 +3141,20 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="4">
+        <v>6.5555251651702452E-5</v>
+      </c>
+      <c r="K20" s="4">
+        <v>3.4393959287596862E-4</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2997,10 +3169,20 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="4">
+        <v>7.4563313736757532E-5</v>
+      </c>
+      <c r="K21" s="4">
+        <v>3.8020975746799328E-4</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3015,10 +3197,20 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="4">
+        <v>7.0051379744719879E-5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>3.4675786902055121E-4</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3033,10 +3225,20 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="4">
+        <v>6.8756943354046399E-5</v>
+      </c>
+      <c r="K23" s="4">
+        <v>4.3034771290308409E-4</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3051,10 +3253,20 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="4">
+        <v>7.474099130033646E-5</v>
+      </c>
+      <c r="K24" s="4">
+        <v>3.2695894120276402E-4</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3069,10 +3281,20 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="4">
+        <v>7.1017033131468205E-5</v>
+      </c>
+      <c r="K25" s="4">
+        <v>4.3996624548749342E-4</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3087,10 +3309,20 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="4">
+        <v>6.3591248191232331E-5</v>
+      </c>
+      <c r="K26" s="4">
+        <v>3.84834694093958E-4</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3105,10 +3337,20 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="4">
+        <v>6.2545507369813662E-5</v>
+      </c>
+      <c r="K27" s="4">
+        <v>5.0684055392800616E-4</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3123,10 +3365,20 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="4">
+        <v>5.8781862659222063E-5</v>
+      </c>
+      <c r="K28" s="4">
+        <v>6.7346392218381522E-4</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3141,10 +3393,20 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="4">
+        <v>6.3310616339789727E-5</v>
+      </c>
+      <c r="K29" s="4">
+        <v>4.883072888603317E-4</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3159,10 +3421,20 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="4">
+        <v>6.0818280722478357E-5</v>
+      </c>
+      <c r="K30" s="4">
+        <v>6.1530994821935576E-4</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3177,10 +3449,20 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="4">
+        <v>6.6338056252489077E-5</v>
+      </c>
+      <c r="K31" s="4">
+        <v>2.668765886594242E-4</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3195,10 +3477,20 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="4">
+        <v>6.6262802899896874E-5</v>
+      </c>
+      <c r="K32" s="4">
+        <v>3.5716331436262401E-4</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3213,10 +3505,20 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="4">
+        <v>7.1605677193336065E-5</v>
+      </c>
+      <c r="K33" s="4">
+        <v>3.2746710305392663E-4</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3231,10 +3533,20 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="4">
+        <v>6.3623174724913829E-5</v>
+      </c>
+      <c r="K34" s="4">
+        <v>5.7007224774734762E-4</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3249,10 +3561,20 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J35" s="4">
+        <v>6.3644385237117667E-5</v>
+      </c>
+      <c r="K35" s="4">
+        <v>4.0948914896583399E-4</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3267,10 +3589,20 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J36" s="4">
+        <v>6.0686476680340451E-5</v>
+      </c>
+      <c r="K36" s="4">
+        <v>6.0989355957949333E-4</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3285,10 +3617,20 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J37" s="4">
+        <v>5.3914538224675222E-5</v>
+      </c>
+      <c r="K37" s="4">
+        <v>7.2623218603174073E-4</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3303,10 +3645,20 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J38" s="4">
+        <v>6.9706177037798836E-5</v>
+      </c>
+      <c r="K38" s="4">
+        <v>3.7374602692075772E-4</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3321,10 +3673,20 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="4">
+        <v>5.847183910739454E-5</v>
+      </c>
+      <c r="K39" s="4">
+        <v>5.0484134207395988E-4</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3339,10 +3701,20 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="4">
+        <v>5.6466837989239277E-5</v>
+      </c>
+      <c r="K40" s="4">
+        <v>5.2298323997494278E-4</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3357,10 +3729,20 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J41" s="4">
+        <v>6.8446815664639565E-5</v>
+      </c>
+      <c r="K41" s="4">
+        <v>3.0002404100116641E-4</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+    </row>
+    <row r="42" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3375,10 +3757,20 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J42" s="4">
+        <v>6.2258534378979718E-5</v>
+      </c>
+      <c r="K42" s="4">
+        <v>4.044777870093374E-4</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+    </row>
+    <row r="43" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3393,10 +3785,20 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J43" s="4">
+        <v>6.7552309498778039E-5</v>
+      </c>
+      <c r="K43" s="4">
+        <v>3.6227537414660119E-4</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+    </row>
+    <row r="44" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3411,10 +3813,20 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J44" s="4">
+        <v>6.6381842477899225E-5</v>
+      </c>
+      <c r="K44" s="4">
+        <v>3.5115267775240658E-4</v>
+      </c>
+      <c r="M44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+    </row>
+    <row r="45" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3429,10 +3841,20 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J45" s="4"/>
-      <c r="K45" s="4"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J45" s="4">
+        <v>6.0905529793870131E-5</v>
+      </c>
+      <c r="K45" s="4">
+        <v>8.3962418889170075E-4</v>
+      </c>
+      <c r="M45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3447,10 +3869,20 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J46" s="4">
+        <v>6.8621935687083105E-5</v>
+      </c>
+      <c r="K46" s="4">
+        <v>2.7880557414886541E-4</v>
+      </c>
+      <c r="M46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+    </row>
+    <row r="47" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3465,10 +3897,20 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J47" s="4">
+        <v>6.277847551087128E-5</v>
+      </c>
+      <c r="K47" s="4">
+        <v>3.6153405812675092E-4</v>
+      </c>
+      <c r="M47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+    </row>
+    <row r="48" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3483,10 +3925,20 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J48" s="4">
+        <v>7.5820951200089224E-5</v>
+      </c>
+      <c r="K48" s="4">
+        <v>4.1705979114878348E-4</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+    </row>
+    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3501,10 +3953,20 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J49" s="4">
+        <v>7.2460149064246712E-5</v>
+      </c>
+      <c r="K49" s="4">
+        <v>3.5708036486013919E-4</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+    </row>
+    <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3519,10 +3981,20 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J50" s="4">
+        <v>6.4655488684721592E-5</v>
+      </c>
+      <c r="K50" s="4">
+        <v>3.0372382159606347E-4</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+    </row>
+    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3537,10 +4009,20 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J51" s="4">
+        <v>6.356089105021878E-5</v>
+      </c>
+      <c r="K51" s="4">
+        <v>4.259217153795682E-4</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+    </row>
+    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3555,10 +4037,20 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J52" s="4">
+        <v>5.4675835871279189E-5</v>
+      </c>
+      <c r="K52" s="4">
+        <v>5.3411667181080149E-4</v>
+      </c>
+      <c r="M52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+    </row>
+    <row r="53" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3573,10 +4065,20 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J53" s="4">
+        <v>6.3701963003330052E-5</v>
+      </c>
+      <c r="K53" s="4">
+        <v>4.4711552840592561E-4</v>
+      </c>
+      <c r="M53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+    </row>
+    <row r="54" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3591,10 +4093,20 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="J54" s="4">
+        <v>6.2834655894844461E-5</v>
+      </c>
+      <c r="K54" s="4">
+        <v>5.0111826616056369E-4</v>
+      </c>
+      <c r="M54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+    </row>
+    <row r="56" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
@@ -3609,16 +4121,27 @@
       <c r="I56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J56" s="4" t="e">
+      <c r="J56" s="4">
         <f>AVERAGE(J5:J54)</f>
+        <v>6.5242363605959167E-5</v>
+      </c>
+      <c r="K56" s="4">
+        <f>AVERAGE(K5:K54)</f>
+        <v>4.4263387461592992E-4</v>
+      </c>
+      <c r="M56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N56" s="4" t="e">
+        <f>AVERAGE(N5:N54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K56" s="4" t="e">
-        <f>AVERAGE(K5:K54)</f>
+      <c r="O56" s="4" t="e">
+        <f>AVERAGE(O5:O54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
@@ -3633,12 +4156,23 @@
       <c r="I57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="4" t="e">
+      <c r="J57" s="4">
         <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>5.3199532644128673E-6</v>
+      </c>
+      <c r="K57" s="4">
+        <f>_xlfn.STDEV.S(K5:K54)</f>
+        <v>1.4792418246170884E-4</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N57" s="4" t="e">
+        <f>_xlfn.STDEV.S(N5:N54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K57" s="4" t="e">
-        <f>_xlfn.STDEV.S(K5:K54)</f>
+      <c r="O57" s="4" t="e">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset-12 test with mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-2.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -2656,7 +2656,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:O57"/>
+  <dimension ref="D3:U57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
@@ -2668,11 +2668,14 @@
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" customWidth="1"/>
+    <col min="20" max="21" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2681,12 +2684,16 @@
         <v>5</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -2701,15 +2708,22 @@
       <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -2728,13 +2742,22 @@
       <c r="K5" s="4">
         <v>3.490213426590818E-4</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O5" s="4">
+        <v>6.538623010137582E-5</v>
+      </c>
+      <c r="P5" s="4">
+        <v>4.310587508338898E-4</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+1</f>
         <v>2</v>
@@ -2755,14 +2778,24 @@
       <c r="K6" s="4">
         <v>3.5510666884648883E-4</v>
       </c>
-      <c r="M6" s="2">
-        <f>M5+1</f>
+      <c r="N6" s="2">
+        <f>N5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O6" s="4">
+        <v>7.0546506736345822E-5</v>
+      </c>
+      <c r="P6" s="4">
+        <v>3.8917484713644947E-4</v>
+      </c>
+      <c r="S6" s="2">
+        <f>S5+1</f>
+        <v>2</v>
+      </c>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <f t="shared" ref="D7:D54" si="0">D6+1</f>
         <v>3</v>
@@ -2783,14 +2816,24 @@
       <c r="K7" s="4">
         <v>4.0006883167582788E-4</v>
       </c>
-      <c r="M7" s="2">
-        <f t="shared" ref="M7:M54" si="2">M6+1</f>
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N54" si="2">N6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O7" s="4">
+        <v>6.7087062734443837E-5</v>
+      </c>
+      <c r="P7" s="4">
+        <v>3.2251299185688743E-4</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" ref="S7:S54" si="3">S6+1</f>
+        <v>3</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2811,14 +2854,24 @@
       <c r="K8" s="4">
         <v>2.9238078911649759E-4</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="4">
+        <v>5.6595738900720797E-5</v>
+      </c>
+      <c r="P8" s="4">
+        <v>6.965897944347843E-4</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2839,14 +2892,24 @@
       <c r="K9" s="4">
         <v>3.9455950933599818E-4</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O9" s="4">
+        <v>6.6602995668214445E-5</v>
+      </c>
+      <c r="P9" s="4">
+        <v>5.0816038430615809E-4</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2867,14 +2930,24 @@
       <c r="K10" s="4">
         <v>2.6907721090905107E-4</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O10" s="4">
+        <v>6.6792134360165389E-5</v>
+      </c>
+      <c r="P10" s="4">
+        <v>6.1767768154050466E-4</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+    </row>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2895,14 +2968,24 @@
       <c r="K11" s="4">
         <v>9.6792392962882865E-4</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O11" s="4">
+        <v>7.2742991543933334E-5</v>
+      </c>
+      <c r="P11" s="4">
+        <v>3.1565493925811688E-4</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+    </row>
+    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2923,14 +3006,24 @@
       <c r="K12" s="4">
         <v>2.8248852689565093E-4</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="4">
+        <v>6.964479015010069E-5</v>
+      </c>
+      <c r="P12" s="4">
+        <v>3.9640863576921321E-4</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2951,14 +3044,24 @@
       <c r="K13" s="4">
         <v>3.5445521812474249E-4</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O13" s="4">
+        <v>6.7864359857989801E-5</v>
+      </c>
+      <c r="P13" s="4">
+        <v>2.7148438703587699E-4</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+    </row>
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2979,14 +3082,24 @@
       <c r="K14" s="4">
         <v>4.4786002296544531E-4</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O14" s="4">
+        <v>6.327687711230646E-5</v>
+      </c>
+      <c r="P14" s="4">
+        <v>5.5851806669042362E-4</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+    </row>
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3007,14 +3120,24 @@
       <c r="K15" s="4">
         <v>4.0671076009897981E-4</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O15" s="4">
+        <v>6.715455015952643E-5</v>
+      </c>
+      <c r="P15" s="4">
+        <v>4.3088132717618798E-4</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+    </row>
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3035,14 +3158,24 @@
       <c r="K16" s="4">
         <v>6.5965253084427386E-4</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O16" s="4">
+        <v>5.4076516890151153E-5</v>
+      </c>
+      <c r="P16" s="4">
+        <v>6.6881330850430921E-4</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3063,14 +3196,24 @@
       <c r="K17" s="4">
         <v>6.6381434295174609E-4</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O17" s="4">
+        <v>7.0843168225786883E-5</v>
+      </c>
+      <c r="P17" s="4">
+        <v>4.1712024740934642E-4</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3091,14 +3234,24 @@
       <c r="K18" s="4">
         <v>3.8840750102423779E-4</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O18" s="4">
+        <v>6.7441056145468558E-5</v>
+      </c>
+      <c r="P18" s="4">
+        <v>4.4083078368546349E-4</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3119,14 +3272,24 @@
       <c r="K19" s="4">
         <v>4.1043540166760571E-4</v>
       </c>
-      <c r="M19" s="2">
+      <c r="N19" s="2">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O19" s="4">
+        <v>7.3673428444633406E-5</v>
+      </c>
+      <c r="P19" s="4">
+        <v>2.814917015854354E-4</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3147,14 +3310,24 @@
       <c r="K20" s="4">
         <v>3.4393959287596862E-4</v>
       </c>
-      <c r="M20" s="2">
+      <c r="N20" s="2">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O20" s="4">
+        <v>6.0021913001854017E-5</v>
+      </c>
+      <c r="P20" s="4">
+        <v>5.0847396013372096E-4</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3175,14 +3348,24 @@
       <c r="K21" s="4">
         <v>3.8020975746799328E-4</v>
       </c>
-      <c r="M21" s="2">
+      <c r="N21" s="2">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O21" s="4">
+        <v>6.9467709441878932E-5</v>
+      </c>
+      <c r="P21" s="4">
+        <v>2.9047013079014881E-4</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3203,14 +3386,24 @@
       <c r="K22" s="4">
         <v>3.4675786902055121E-4</v>
       </c>
-      <c r="M22" s="2">
+      <c r="N22" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O22" s="4">
+        <v>6.8801834612356068E-5</v>
+      </c>
+      <c r="P22" s="4">
+        <v>4.7788074581502608E-4</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3231,14 +3424,24 @@
       <c r="K23" s="4">
         <v>4.3034771290308409E-4</v>
       </c>
-      <c r="M23" s="2">
+      <c r="N23" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O23" s="4">
+        <v>7.3687089909426476E-5</v>
+      </c>
+      <c r="P23" s="4">
+        <v>3.9659126114944502E-4</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3259,14 +3462,24 @@
       <c r="K24" s="4">
         <v>3.2695894120276402E-4</v>
       </c>
-      <c r="M24" s="2">
+      <c r="N24" s="2">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O24" s="4">
+        <v>7.1325688919946168E-5</v>
+      </c>
+      <c r="P24" s="4">
+        <v>5.3024167099257995E-4</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3287,14 +3500,24 @@
       <c r="K25" s="4">
         <v>4.3996624548749342E-4</v>
       </c>
-      <c r="M25" s="2">
+      <c r="N25" s="2">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O25" s="4">
+        <v>6.7259592183422661E-5</v>
+      </c>
+      <c r="P25" s="4">
+        <v>5.020710797557944E-4</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3315,14 +3538,24 @@
       <c r="K26" s="4">
         <v>3.84834694093958E-4</v>
       </c>
-      <c r="M26" s="2">
+      <c r="N26" s="2">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O26" s="4">
+        <v>7.4354861481249333E-5</v>
+      </c>
+      <c r="P26" s="4">
+        <v>3.1187093810236858E-4</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3343,14 +3576,24 @@
       <c r="K27" s="4">
         <v>5.0684055392800616E-4</v>
       </c>
-      <c r="M27" s="2">
+      <c r="N27" s="2">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O27" s="4">
+        <v>5.6743312526181518E-5</v>
+      </c>
+      <c r="P27" s="4">
+        <v>6.4325740100790901E-4</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3371,14 +3614,24 @@
       <c r="K28" s="4">
         <v>6.7346392218381522E-4</v>
       </c>
-      <c r="M28" s="2">
+      <c r="N28" s="2">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O28" s="4">
+        <v>6.5621086574923311E-5</v>
+      </c>
+      <c r="P28" s="4">
+        <v>3.105464889056784E-4</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3399,14 +3652,24 @@
       <c r="K29" s="4">
         <v>4.883072888603317E-4</v>
       </c>
-      <c r="M29" s="2">
+      <c r="N29" s="2">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O29" s="4">
+        <v>6.9420212575131268E-5</v>
+      </c>
+      <c r="P29" s="4">
+        <v>3.265691995771626E-4</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3427,14 +3690,24 @@
       <c r="K30" s="4">
         <v>6.1530994821935576E-4</v>
       </c>
-      <c r="M30" s="2">
+      <c r="N30" s="2">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O30" s="4">
+        <v>6.759822095948801E-5</v>
+      </c>
+      <c r="P30" s="4">
+        <v>2.182215377937837E-4</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3455,14 +3728,24 @@
       <c r="K31" s="4">
         <v>2.668765886594242E-4</v>
       </c>
-      <c r="M31" s="2">
+      <c r="N31" s="2">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O31" s="4">
+        <v>7.0889028803121108E-5</v>
+      </c>
+      <c r="P31" s="4">
+        <v>3.1359733988687688E-4</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3483,14 +3766,24 @@
       <c r="K32" s="4">
         <v>3.5716331436262401E-4</v>
       </c>
-      <c r="M32" s="2">
+      <c r="N32" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O32" s="4">
+        <v>6.9111602008266475E-5</v>
+      </c>
+      <c r="P32" s="4">
+        <v>4.3127574069457952E-4</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+    </row>
+    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3511,14 +3804,24 @@
       <c r="K33" s="4">
         <v>3.2746710305392663E-4</v>
       </c>
-      <c r="M33" s="2">
+      <c r="N33" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="4">
+        <v>6.0977680521973533E-5</v>
+      </c>
+      <c r="P33" s="4">
+        <v>5.4006720626730009E-4</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+    </row>
+    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3539,14 +3842,24 @@
       <c r="K34" s="4">
         <v>5.7007224774734762E-4</v>
       </c>
-      <c r="M34" s="2">
+      <c r="N34" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-    </row>
-    <row r="35" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="4">
+        <v>6.3057373410104002E-5</v>
+      </c>
+      <c r="P34" s="4">
+        <v>5.1163303853720885E-4</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+    </row>
+    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3567,14 +3880,24 @@
       <c r="K35" s="4">
         <v>4.0948914896583399E-4</v>
       </c>
-      <c r="M35" s="2">
+      <c r="N35" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O35" s="4">
+        <v>7.271291761514178E-5</v>
+      </c>
+      <c r="P35" s="4">
+        <v>3.3589957362755492E-4</v>
+      </c>
+      <c r="S35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="T35" s="4"/>
+      <c r="U35" s="4"/>
+    </row>
+    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3595,14 +3918,24 @@
       <c r="K36" s="4">
         <v>6.0989355957949333E-4</v>
       </c>
-      <c r="M36" s="2">
+      <c r="N36" s="2">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O36" s="4">
+        <v>7.4784207580338885E-5</v>
+      </c>
+      <c r="P36" s="4">
+        <v>4.731431736434188E-4</v>
+      </c>
+      <c r="S36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+    </row>
+    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3623,14 +3956,24 @@
       <c r="K37" s="4">
         <v>7.2623218603174073E-4</v>
       </c>
-      <c r="M37" s="2">
+      <c r="N37" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-    </row>
-    <row r="38" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="4">
+        <v>6.2874727781176898E-5</v>
+      </c>
+      <c r="P37" s="4">
+        <v>7.5807896276420335E-4</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+    </row>
+    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3651,14 +3994,24 @@
       <c r="K38" s="4">
         <v>3.7374602692075772E-4</v>
       </c>
-      <c r="M38" s="2">
+      <c r="N38" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O38" s="4">
+        <v>7.2983643456188724E-5</v>
+      </c>
+      <c r="P38" s="4">
+        <v>3.7619908514019608E-4</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+    </row>
+    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3679,14 +4032,24 @@
       <c r="K39" s="4">
         <v>5.0484134207395988E-4</v>
       </c>
-      <c r="M39" s="2">
+      <c r="N39" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-    </row>
-    <row r="40" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="4">
+        <v>6.6765231473324492E-5</v>
+      </c>
+      <c r="P39" s="4">
+        <v>3.7814051363257788E-4</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+    </row>
+    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3707,14 +4070,24 @@
       <c r="K40" s="4">
         <v>5.2298323997494278E-4</v>
       </c>
-      <c r="M40" s="2">
+      <c r="N40" s="2">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O40" s="4">
+        <v>6.4680813988119174E-5</v>
+      </c>
+      <c r="P40" s="4">
+        <v>5.659293919582256E-4</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+    </row>
+    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3735,14 +4108,24 @@
       <c r="K41" s="4">
         <v>3.0002404100116641E-4</v>
       </c>
-      <c r="M41" s="2">
+      <c r="N41" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O41" s="4">
+        <v>5.8963275451774682E-5</v>
+      </c>
+      <c r="P41" s="4">
+        <v>7.7936473310642144E-4</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+    </row>
+    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3763,14 +4146,24 @@
       <c r="K42" s="4">
         <v>4.044777870093374E-4</v>
       </c>
-      <c r="M42" s="2">
+      <c r="N42" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-    </row>
-    <row r="43" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O42" s="4">
+        <v>7.0917133990268261E-5</v>
+      </c>
+      <c r="P42" s="4">
+        <v>3.2938554333627898E-4</v>
+      </c>
+      <c r="S42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+    </row>
+    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3791,14 +4184,24 @@
       <c r="K43" s="4">
         <v>3.6227537414660119E-4</v>
       </c>
-      <c r="M43" s="2">
+      <c r="N43" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O43" s="4">
+        <v>6.297620094941374E-5</v>
+      </c>
+      <c r="P43" s="4">
+        <v>4.7179575914176611E-4</v>
+      </c>
+      <c r="S43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+    </row>
+    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3819,14 +4222,24 @@
       <c r="K44" s="4">
         <v>3.5115267775240658E-4</v>
       </c>
-      <c r="M44" s="2">
+      <c r="N44" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O44" s="4">
+        <v>7.1092019292882277E-5</v>
+      </c>
+      <c r="P44" s="4">
+        <v>2.9597664387176828E-4</v>
+      </c>
+      <c r="S44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+    </row>
+    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3847,14 +4260,24 @@
       <c r="K45" s="4">
         <v>8.3962418889170075E-4</v>
       </c>
-      <c r="M45" s="2">
+      <c r="N45" s="2">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-    </row>
-    <row r="46" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O45" s="4">
+        <v>7.0747564249598182E-5</v>
+      </c>
+      <c r="P45" s="4">
+        <v>2.133542633564671E-4</v>
+      </c>
+      <c r="S45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+    </row>
+    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3875,14 +4298,24 @@
       <c r="K46" s="4">
         <v>2.7880557414886541E-4</v>
       </c>
-      <c r="M46" s="2">
+      <c r="N46" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O46" s="4">
+        <v>6.9974846186893482E-5</v>
+      </c>
+      <c r="P46" s="4">
+        <v>3.6492817820061078E-4</v>
+      </c>
+      <c r="S46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+    </row>
+    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3903,14 +4336,24 @@
       <c r="K47" s="4">
         <v>3.6153405812675092E-4</v>
       </c>
-      <c r="M47" s="2">
+      <c r="N47" s="2">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-    </row>
-    <row r="48" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O47" s="4">
+        <v>7.3129826632839759E-5</v>
+      </c>
+      <c r="P47" s="4">
+        <v>4.7262986587515518E-4</v>
+      </c>
+      <c r="S47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+    </row>
+    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3931,14 +4374,24 @@
       <c r="K48" s="4">
         <v>4.1705979114878348E-4</v>
       </c>
-      <c r="M48" s="2">
+      <c r="N48" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-    </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O48" s="4">
+        <v>7.1120880516784184E-5</v>
+      </c>
+      <c r="P48" s="4">
+        <v>3.9564066074949407E-4</v>
+      </c>
+      <c r="S48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+    </row>
+    <row r="49" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3959,14 +4412,24 @@
       <c r="K49" s="4">
         <v>3.5708036486013919E-4</v>
       </c>
-      <c r="M49" s="2">
+      <c r="N49" s="2">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-    </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O49" s="4">
+        <v>6.8928106676395448E-5</v>
+      </c>
+      <c r="P49" s="4">
+        <v>5.4101197042607347E-4</v>
+      </c>
+      <c r="S49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+    </row>
+    <row r="50" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3987,14 +4450,24 @@
       <c r="K50" s="4">
         <v>3.0372382159606347E-4</v>
       </c>
-      <c r="M50" s="2">
+      <c r="N50" s="2">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-    </row>
-    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O50" s="4">
+        <v>6.9048013942346633E-5</v>
+      </c>
+      <c r="P50" s="4">
+        <v>5.3495834419230658E-4</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+    </row>
+    <row r="51" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4015,14 +4488,24 @@
       <c r="K51" s="4">
         <v>4.259217153795682E-4</v>
       </c>
-      <c r="M51" s="2">
+      <c r="N51" s="2">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-    </row>
-    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O51" s="4">
+        <v>6.8503170848396592E-5</v>
+      </c>
+      <c r="P51" s="4">
+        <v>4.1499896036886589E-4</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+    </row>
+    <row r="52" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4043,14 +4526,24 @@
       <c r="K52" s="4">
         <v>5.3411667181080149E-4</v>
       </c>
-      <c r="M52" s="2">
+      <c r="N52" s="2">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="4"/>
-      <c r="O52" s="4"/>
-    </row>
-    <row r="53" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O52" s="4">
+        <v>7.5145814766653437E-5</v>
+      </c>
+      <c r="P52" s="4">
+        <v>4.6804487821653268E-4</v>
+      </c>
+      <c r="S52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+    </row>
+    <row r="53" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4071,14 +4564,24 @@
       <c r="K53" s="4">
         <v>4.4711552840592561E-4</v>
       </c>
-      <c r="M53" s="2">
+      <c r="N53" s="2">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-    </row>
-    <row r="54" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O53" s="4">
+        <v>6.9338186237967667E-5</v>
+      </c>
+      <c r="P53" s="4">
+        <v>3.6529660253169428E-4</v>
+      </c>
+      <c r="S53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+    </row>
+    <row r="54" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4099,14 +4602,24 @@
       <c r="K54" s="4">
         <v>5.0111826616056369E-4</v>
       </c>
-      <c r="M54" s="2">
+      <c r="N54" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-    </row>
-    <row r="56" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O54" s="4">
+        <v>6.9400229889560994E-5</v>
+      </c>
+      <c r="P54" s="4">
+        <v>4.0656552993898322E-4</v>
+      </c>
+      <c r="S54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+    </row>
+    <row r="56" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>2</v>
       </c>
@@ -4129,19 +4642,30 @@
         <f>AVERAGE(K5:K54)</f>
         <v>4.4263387461592992E-4</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="N56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N56" s="4" t="e">
-        <f>AVERAGE(N5:N54)</f>
+      <c r="O56" s="4">
+        <f>AVERAGE(O5:O54)</f>
+        <v>6.784304850973103E-5</v>
+      </c>
+      <c r="P56" s="4">
+        <f>AVERAGE(P5:P54)</f>
+        <v>4.4000976441422457E-4</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T56" s="4" t="e">
+        <f>AVERAGE(T5:T54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O56" s="4" t="e">
-        <f>AVERAGE(O5:O54)</f>
+      <c r="U56" s="4" t="e">
+        <f>AVERAGE(U5:U54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>3</v>
       </c>
@@ -4164,15 +4688,26 @@
         <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>1.4792418246170884E-4</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="N57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N57" s="4" t="e">
-        <f>_xlfn.STDEV.S(N5:N54)</f>
+      <c r="O57" s="4">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>4.8636923970691848E-6</v>
+      </c>
+      <c r="P57" s="4">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>1.3092343137863344E-4</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T57" s="4" t="e">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O57" s="4" t="e">
-        <f>_xlfn.STDEV.S(O5:O54)</f>
+      <c r="U57" s="4" t="e">
+        <f>_xlfn.STDEV.S(U5:U54)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
superdataset-13 test with mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-2.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-2.xlsx
@@ -2658,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,8 +2754,12 @@
       <c r="S5" s="2">
         <v>1</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
+      <c r="T5" s="4">
+        <v>5.503011245186134E-5</v>
+      </c>
+      <c r="U5" s="4">
+        <v>8.3540650792029026E-4</v>
+      </c>
     </row>
     <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
@@ -2792,8 +2796,12 @@
         <f>S5+1</f>
         <v>2</v>
       </c>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
+      <c r="T6" s="4">
+        <v>5.9967451738382029E-5</v>
+      </c>
+      <c r="U6" s="4">
+        <v>3.7823060819885398E-4</v>
+      </c>
     </row>
     <row r="7" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
@@ -2830,8 +2838,12 @@
         <f t="shared" ref="S7:S54" si="3">S6+1</f>
         <v>3</v>
       </c>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
+      <c r="T7" s="4">
+        <v>5.2591582908256337E-5</v>
+      </c>
+      <c r="U7" s="4">
+        <v>6.1545257336610053E-4</v>
+      </c>
     </row>
     <row r="8" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
@@ -2868,8 +2880,12 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
+      <c r="T8" s="4">
+        <v>6.3097607068156441E-5</v>
+      </c>
+      <c r="U8" s="4">
+        <v>3.1850768399081672E-4</v>
+      </c>
     </row>
     <row r="9" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
@@ -2906,8 +2922,12 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
+      <c r="T9" s="4">
+        <v>6.651413183117218E-5</v>
+      </c>
+      <c r="U9" s="4">
+        <v>3.9108209196853691E-4</v>
+      </c>
     </row>
     <row r="10" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
@@ -2944,8 +2964,12 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
+      <c r="T10" s="4">
+        <v>5.6136414158981842E-5</v>
+      </c>
+      <c r="U10" s="4">
+        <v>4.6807925904620537E-4</v>
+      </c>
     </row>
     <row r="11" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
@@ -2982,8 +3006,12 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
+      <c r="T11" s="4">
+        <v>5.9176816500790682E-5</v>
+      </c>
+      <c r="U11" s="4">
+        <v>4.2690692371642752E-4</v>
+      </c>
     </row>
     <row r="12" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
@@ -3020,8 +3048,12 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
+      <c r="T12" s="4">
+        <v>5.3486824799421879E-5</v>
+      </c>
+      <c r="U12" s="4">
+        <v>6.2754703219099824E-4</v>
+      </c>
     </row>
     <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
@@ -3058,8 +3090,12 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
+      <c r="T13" s="4">
+        <v>6.4052016992818749E-5</v>
+      </c>
+      <c r="U13" s="4">
+        <v>3.6169760037931009E-4</v>
+      </c>
     </row>
     <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
@@ -3096,8 +3132,12 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
+      <c r="T14" s="4">
+        <v>7.244650571687623E-5</v>
+      </c>
+      <c r="U14" s="4">
+        <v>3.3460575962597901E-4</v>
+      </c>
     </row>
     <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
@@ -3134,8 +3174,12 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
+      <c r="T15" s="4">
+        <v>5.8788226974038367E-5</v>
+      </c>
+      <c r="U15" s="4">
+        <v>5.3558070035386682E-4</v>
+      </c>
     </row>
     <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
@@ -3172,8 +3216,12 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
+      <c r="T16" s="4">
+        <v>6.4415858830368177E-5</v>
+      </c>
+      <c r="U16" s="4">
+        <v>5.0167872385648601E-4</v>
+      </c>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
@@ -3210,8 +3258,12 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
+      <c r="T17" s="4">
+        <v>7.1043242439360123E-5</v>
+      </c>
+      <c r="U17" s="4">
+        <v>3.0788156582625838E-4</v>
+      </c>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
@@ -3248,8 +3300,12 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
+      <c r="T18" s="4">
+        <v>6.2696668505210143E-5</v>
+      </c>
+      <c r="U18" s="4">
+        <v>3.2990491081884331E-4</v>
+      </c>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
@@ -3286,8 +3342,12 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
+      <c r="T19" s="4">
+        <v>6.587384557238129E-5</v>
+      </c>
+      <c r="U19" s="4">
+        <v>4.4467908621744271E-4</v>
+      </c>
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
@@ -3324,8 +3384,12 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
+      <c r="T20" s="4">
+        <v>6.8778554865638961E-5</v>
+      </c>
+      <c r="U20" s="4">
+        <v>3.2966716429677341E-4</v>
+      </c>
     </row>
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
@@ -3362,8 +3426,12 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
+      <c r="T21" s="4">
+        <v>6.1696713670308831E-5</v>
+      </c>
+      <c r="U21" s="4">
+        <v>6.1832939730611892E-4</v>
+      </c>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
@@ -3400,8 +3468,12 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
+      <c r="T22" s="4">
+        <v>6.2271385162116001E-5</v>
+      </c>
+      <c r="U22" s="4">
+        <v>4.9750038377983051E-4</v>
+      </c>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
@@ -3438,8 +3510,12 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
+      <c r="T23" s="4">
+        <v>6.6534327743237738E-5</v>
+      </c>
+      <c r="U23" s="4">
+        <v>3.9604336967912737E-4</v>
+      </c>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
@@ -3476,8 +3552,12 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
+      <c r="T24" s="4">
+        <v>6.7953094678194638E-5</v>
+      </c>
+      <c r="U24" s="4">
+        <v>2.9339056320201859E-4</v>
+      </c>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
@@ -3514,8 +3594,12 @@
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
+      <c r="T25" s="4">
+        <v>6.3636899634327115E-5</v>
+      </c>
+      <c r="U25" s="4">
+        <v>3.6736937705477199E-4</v>
+      </c>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
@@ -3552,8 +3636,12 @@
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
+      <c r="T26" s="4">
+        <v>5.5042517614221591E-5</v>
+      </c>
+      <c r="U26" s="4">
+        <v>4.8190988349849212E-4</v>
+      </c>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
@@ -3590,8 +3678,12 @@
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
+      <c r="T27" s="4">
+        <v>6.1508612493463589E-5</v>
+      </c>
+      <c r="U27" s="4">
+        <v>3.730815843846586E-4</v>
+      </c>
     </row>
     <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
@@ -3628,8 +3720,12 @@
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
+      <c r="T28" s="4">
+        <v>6.5575908474247891E-5</v>
+      </c>
+      <c r="U28" s="4">
+        <v>4.3861615287973032E-4</v>
+      </c>
     </row>
     <row r="29" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
@@ -3666,8 +3762,12 @@
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
+      <c r="T29" s="4">
+        <v>5.3472650915101847E-5</v>
+      </c>
+      <c r="U29" s="4">
+        <v>6.6416436890334306E-4</v>
+      </c>
     </row>
     <row r="30" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
@@ -3704,8 +3804,12 @@
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
+      <c r="T30" s="4">
+        <v>5.589026740771058E-5</v>
+      </c>
+      <c r="U30" s="4">
+        <v>5.6239866346945719E-4</v>
+      </c>
     </row>
     <row r="31" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
@@ -3742,8 +3846,12 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
+      <c r="T31" s="4">
+        <v>6.0667109582902133E-5</v>
+      </c>
+      <c r="U31" s="4">
+        <v>3.4072890349385432E-4</v>
+      </c>
     </row>
     <row r="32" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
@@ -3780,8 +3888,12 @@
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
+      <c r="T32" s="4">
+        <v>6.4819447104103053E-5</v>
+      </c>
+      <c r="U32" s="4">
+        <v>5.1475647798412971E-4</v>
+      </c>
     </row>
     <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
@@ -3818,8 +3930,12 @@
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
+      <c r="T33" s="4">
+        <v>5.7980135711774843E-5</v>
+      </c>
+      <c r="U33" s="4">
+        <v>6.6343539150521451E-4</v>
+      </c>
     </row>
     <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
@@ -3856,8 +3972,12 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
+      <c r="T34" s="4">
+        <v>6.2409254788756301E-5</v>
+      </c>
+      <c r="U34" s="4">
+        <v>4.5863123904253602E-4</v>
+      </c>
     </row>
     <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
@@ -3894,8 +4014,12 @@
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
+      <c r="T35" s="4">
+        <v>5.7053680281262648E-5</v>
+      </c>
+      <c r="U35" s="4">
+        <v>5.9131996851791613E-4</v>
+      </c>
     </row>
     <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
@@ -3932,8 +4056,12 @@
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
+      <c r="T36" s="4">
+        <v>5.9313111471295708E-5</v>
+      </c>
+      <c r="U36" s="4">
+        <v>3.0412926905250672E-4</v>
+      </c>
     </row>
     <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
@@ -3970,8 +4098,12 @@
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
+      <c r="T37" s="4">
+        <v>5.8873679508800583E-5</v>
+      </c>
+      <c r="U37" s="4">
+        <v>4.9599222719775053E-4</v>
+      </c>
     </row>
     <row r="38" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
@@ -4008,8 +4140,12 @@
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
+      <c r="T38" s="4">
+        <v>6.7396970948967267E-5</v>
+      </c>
+      <c r="U38" s="4">
+        <v>3.0102327399908512E-4</v>
+      </c>
     </row>
     <row r="39" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
@@ -4046,8 +4182,12 @@
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
+      <c r="T39" s="4">
+        <v>6.6479926343178161E-5</v>
+      </c>
+      <c r="U39" s="4">
+        <v>4.2070986772552578E-4</v>
+      </c>
     </row>
     <row r="40" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
@@ -4084,8 +4224,12 @@
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
+      <c r="T40" s="4">
+        <v>5.7016136681753607E-5</v>
+      </c>
+      <c r="U40" s="4">
+        <v>4.3018509130313381E-4</v>
+      </c>
     </row>
     <row r="41" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
@@ -4122,8 +4266,12 @@
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
+      <c r="T41" s="4">
+        <v>6.2959941453997841E-5</v>
+      </c>
+      <c r="U41" s="4">
+        <v>7.8432089532466838E-4</v>
+      </c>
     </row>
     <row r="42" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
@@ -4160,8 +4308,12 @@
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="T42" s="4"/>
-      <c r="U42" s="4"/>
+      <c r="T42" s="4">
+        <v>5.3312671823951763E-5</v>
+      </c>
+      <c r="U42" s="4">
+        <v>5.9893724041657501E-4</v>
+      </c>
     </row>
     <row r="43" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
@@ -4198,8 +4350,12 @@
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
+      <c r="T43" s="4">
+        <v>6.0662792959156002E-5</v>
+      </c>
+      <c r="U43" s="4">
+        <v>5.3786702840837529E-4</v>
+      </c>
     </row>
     <row r="44" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
@@ -4236,8 +4392,12 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
+      <c r="T44" s="4">
+        <v>6.0029534792445907E-5</v>
+      </c>
+      <c r="U44" s="4">
+        <v>6.6301868090244014E-4</v>
+      </c>
     </row>
     <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
@@ -4274,8 +4434,12 @@
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
+      <c r="T45" s="4">
+        <v>6.7094581281543304E-5</v>
+      </c>
+      <c r="U45" s="4">
+        <v>3.9966658594246812E-4</v>
+      </c>
     </row>
     <row r="46" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
@@ -4312,8 +4476,12 @@
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
+      <c r="T46" s="4">
+        <v>6.5098897339210227E-5</v>
+      </c>
+      <c r="U46" s="4">
+        <v>4.0487964608311103E-4</v>
+      </c>
     </row>
     <row r="47" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
@@ -4350,8 +4518,12 @@
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
+      <c r="T47" s="4">
+        <v>5.9981150841951513E-5</v>
+      </c>
+      <c r="U47" s="4">
+        <v>5.1727586868207873E-4</v>
+      </c>
     </row>
     <row r="48" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
@@ -4388,8 +4560,12 @@
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
+      <c r="T48" s="4">
+        <v>6.1855361938343333E-5</v>
+      </c>
+      <c r="U48" s="4">
+        <v>3.6377727648352062E-4</v>
+      </c>
     </row>
     <row r="49" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
@@ -4426,8 +4602,12 @@
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
+      <c r="T49" s="4">
+        <v>6.7824709597586656E-5</v>
+      </c>
+      <c r="U49" s="4">
+        <v>5.1329421531259357E-4</v>
+      </c>
     </row>
     <row r="50" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
@@ -4464,8 +4644,12 @@
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="T50" s="4"/>
-      <c r="U50" s="4"/>
+      <c r="T50" s="4">
+        <v>5.4776555583699901E-5</v>
+      </c>
+      <c r="U50" s="4">
+        <v>5.9226057513606469E-4</v>
+      </c>
     </row>
     <row r="51" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
@@ -4502,8 +4686,12 @@
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="T51" s="4"/>
-      <c r="U51" s="4"/>
+      <c r="T51" s="4">
+        <v>6.5138314692705338E-5</v>
+      </c>
+      <c r="U51" s="4">
+        <v>2.8794104521623012E-4</v>
+      </c>
     </row>
     <row r="52" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
@@ -4540,8 +4728,12 @@
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="T52" s="4"/>
-      <c r="U52" s="4"/>
+      <c r="T52" s="4">
+        <v>6.2254630953650577E-5</v>
+      </c>
+      <c r="U52" s="4">
+        <v>3.8433863290953388E-4</v>
+      </c>
     </row>
     <row r="53" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
@@ -4578,8 +4770,12 @@
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="T53" s="4"/>
-      <c r="U53" s="4"/>
+      <c r="T53" s="4">
+        <v>6.4450193365712664E-5</v>
+      </c>
+      <c r="U53" s="4">
+        <v>3.3611032757183942E-4</v>
+      </c>
     </row>
     <row r="54" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
@@ -4616,8 +4812,12 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="T54" s="4"/>
-      <c r="U54" s="4"/>
+      <c r="T54" s="4">
+        <v>6.1309046924711992E-5</v>
+      </c>
+      <c r="U54" s="4">
+        <v>3.363964903392386E-4</v>
+      </c>
     </row>
     <row r="56" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
@@ -4656,13 +4856,13 @@
       <c r="S56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T56" s="4" t="e">
+      <c r="T56" s="4">
         <f>AVERAGE(T5:T54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U56" s="4" t="e">
+        <v>6.172872150236213E-5</v>
+      </c>
+      <c r="U56" s="4">
         <f>AVERAGE(U5:U54)</f>
-        <v>#DIV/0!</v>
+        <v>4.6281416308962262E-4</v>
       </c>
     </row>
     <row r="57" spans="4:21" x14ac:dyDescent="0.25">
@@ -4702,13 +4902,13 @@
       <c r="S57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="T57" s="4" t="e">
+      <c r="T57" s="4">
         <f>_xlfn.STDEV.S(T5:T54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U57" s="4" t="e">
+        <v>4.8292468090712797E-6</v>
+      </c>
+      <c r="U57" s="4">
         <f>_xlfn.STDEV.S(U5:U54)</f>
-        <v>#DIV/0!</v>
+        <v>1.3166928503285182E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test without consnewarea feature
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-2.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="MAE" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -50,6 +50,21 @@
   </si>
   <si>
     <t>test (MSE)</t>
+  </si>
+  <si>
+    <t>train avg</t>
+  </si>
+  <si>
+    <t>test avg</t>
+  </si>
+  <si>
+    <t>set-00</t>
+  </si>
+  <si>
+    <t>set-10</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-13.csv without consnewareas)</t>
   </si>
 </sst>
 </file>
@@ -103,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -113,6 +128,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -130,6 +148,1003 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MAE!$E$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>train avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>MAE!$F$62:$G$62</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>set-00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>set-10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MAE!$F$63:$G$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>114.07751352160854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>102.39860418480858</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-21BD-4037-8C03-43574794BFE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>MAE!$E$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>MAE!$F$62:$G$62</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>set-00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>set-10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>MAE!$F$64:$G$64</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>303.82919657827125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>274.36524332688504</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-21BD-4037-8C03-43574794BFE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="37216"/>
+        <c:axId val="31808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="37216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="31808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:T57"/>
+  <dimension ref="C3:X64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA28" sqref="AA28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,9 +1426,11 @@
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
     <col min="19" max="19" width="14.5703125" customWidth="1"/>
     <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -430,8 +1447,12 @@
         <v>7</v>
       </c>
       <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -460,8 +1481,15 @@
       <c r="T4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V4" s="2"/>
+      <c r="W4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -498,8 +1526,17 @@
       <c r="T5" s="3">
         <v>274.65105899419649</v>
       </c>
-    </row>
-    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V5" s="2">
+        <v>1</v>
+      </c>
+      <c r="W5" s="3">
+        <v>101.8925447508463</v>
+      </c>
+      <c r="X5" s="3">
+        <v>318.25632978723331</v>
+      </c>
+    </row>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -540,8 +1577,18 @@
       <c r="T6" s="3">
         <v>300.48460831721388</v>
       </c>
-    </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V6" s="2">
+        <f>V5+1</f>
+        <v>2</v>
+      </c>
+      <c r="W6" s="3">
+        <v>101.8975145137878</v>
+      </c>
+      <c r="X6" s="3">
+        <v>310.57984042553107</v>
+      </c>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -582,8 +1629,18 @@
       <c r="T7" s="3">
         <v>297.76296905222358</v>
       </c>
-    </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V7" s="2">
+        <f t="shared" ref="V7:V54" si="4">V6+1</f>
+        <v>3</v>
+      </c>
+      <c r="W7" s="3">
+        <v>100.9329583938071</v>
+      </c>
+      <c r="X7" s="3">
+        <v>317.25941005802628</v>
+      </c>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -624,8 +1681,18 @@
       <c r="T8" s="3">
         <v>273.04195841392573</v>
       </c>
-    </row>
-    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V8" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="W8" s="3">
+        <v>105.3882619738749</v>
+      </c>
+      <c r="X8" s="3">
+        <v>273.69427949709791</v>
+      </c>
+    </row>
+    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -666,8 +1733,18 @@
       <c r="T9" s="3">
         <v>257.82382978723319</v>
       </c>
-    </row>
-    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V9" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="W9" s="3">
+        <v>102.8637977745522</v>
+      </c>
+      <c r="X9" s="3">
+        <v>260.77474854932223</v>
+      </c>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -708,8 +1785,18 @@
       <c r="T10" s="3">
         <v>287.40967601547311</v>
       </c>
-    </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V10" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="W10" s="3">
+        <v>104.3771480406383</v>
+      </c>
+      <c r="X10" s="3">
+        <v>273.28678916827772</v>
+      </c>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -750,8 +1837,18 @@
       <c r="T11" s="3">
         <v>258.10086073500901</v>
       </c>
-    </row>
-    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V11" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="W11" s="3">
+        <v>104.6761357039184</v>
+      </c>
+      <c r="X11" s="3">
+        <v>266.31502417794889</v>
+      </c>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -792,8 +1889,18 @@
       <c r="T12" s="3">
         <v>291.49372340425452</v>
       </c>
-    </row>
-    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V12" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="W12" s="3">
+        <v>105.4959470246731</v>
+      </c>
+      <c r="X12" s="3">
+        <v>284.74496615086957</v>
+      </c>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -834,8 +1941,18 @@
       <c r="T13" s="3">
         <v>270.54553191489282</v>
       </c>
-    </row>
-    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V13" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="W13" s="3">
+        <v>105.5399419448473</v>
+      </c>
+      <c r="X13" s="3">
+        <v>251.92776112185609</v>
+      </c>
+    </row>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -876,8 +1993,18 @@
       <c r="T14" s="3">
         <v>261.10185686653688</v>
       </c>
-    </row>
-    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V14" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="W14" s="3">
+        <v>102.200432994678</v>
+      </c>
+      <c r="X14" s="3">
+        <v>278.798597678916</v>
+      </c>
+    </row>
+    <row r="15" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -918,8 +2045,18 @@
       <c r="T15" s="3">
         <v>262.31161025144991</v>
       </c>
-    </row>
-    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V15" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="W15" s="3">
+        <v>105.1113909046925</v>
+      </c>
+      <c r="X15" s="3">
+        <v>289.79151353965102</v>
+      </c>
+    </row>
+    <row r="16" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -960,8 +2097,18 @@
       <c r="T16" s="3">
         <v>297.60948259187529</v>
       </c>
-    </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V16" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="W16" s="3">
+        <v>103.0311393323655</v>
+      </c>
+      <c r="X16" s="3">
+        <v>281.11529980657548</v>
+      </c>
+    </row>
+    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1002,8 +2149,18 @@
       <c r="T17" s="3">
         <v>274.84925048355819</v>
       </c>
-    </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V17" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="W17" s="3">
+        <v>104.1702503628444</v>
+      </c>
+      <c r="X17" s="3">
+        <v>286.98130077369348</v>
+      </c>
+    </row>
+    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1044,8 +2201,18 @@
       <c r="T18" s="3">
         <v>280.11029013539581</v>
       </c>
-    </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V18" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="W18" s="3">
+        <v>103.72333696178001</v>
+      </c>
+      <c r="X18" s="3">
+        <v>299.83950193423522</v>
+      </c>
+    </row>
+    <row r="19" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1086,8 +2253,18 @@
       <c r="T19" s="3">
         <v>252.58670212765881</v>
       </c>
-    </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V19" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="W19" s="3">
+        <v>102.1496686018381</v>
+      </c>
+      <c r="X19" s="3">
+        <v>316.64463249516359</v>
+      </c>
+    </row>
+    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1128,8 +2305,18 @@
       <c r="T20" s="3">
         <v>277.7396663442932</v>
       </c>
-    </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V20" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="W20" s="3">
+        <v>104.085245524915</v>
+      </c>
+      <c r="X20" s="3">
+        <v>293.20878626692371</v>
+      </c>
+    </row>
+    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1170,8 +2357,18 @@
       <c r="T21" s="3">
         <v>271.45968085106301</v>
       </c>
-    </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V21" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="W21" s="3">
+        <v>105.463474842767</v>
+      </c>
+      <c r="X21" s="3">
+        <v>260.21929883945762</v>
+      </c>
+    </row>
+    <row r="22" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1212,8 +2409,18 @@
       <c r="T22" s="3">
         <v>280.84002417794892</v>
       </c>
-    </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V22" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="W22" s="3">
+        <v>107.6748246250602</v>
+      </c>
+      <c r="X22" s="3">
+        <v>224.0764023210823</v>
+      </c>
+    </row>
+    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1254,8 +2461,18 @@
       <c r="T23" s="3">
         <v>293.74333655705908</v>
       </c>
-    </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V23" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="W23" s="3">
+        <v>101.4250483792934</v>
+      </c>
+      <c r="X23" s="3">
+        <v>274.86751934235889</v>
+      </c>
+    </row>
+    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1296,8 +2513,18 @@
       <c r="T24" s="3">
         <v>282.72618955512479</v>
       </c>
-    </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V24" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="W24" s="3">
+        <v>104.4872895500723</v>
+      </c>
+      <c r="X24" s="3">
+        <v>291.20140232108253</v>
+      </c>
+    </row>
+    <row r="25" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1338,8 +2565,18 @@
       <c r="T25" s="3">
         <v>257.92569632495082</v>
       </c>
-    </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V25" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="W25" s="3">
+        <v>101.90096274794359</v>
+      </c>
+      <c r="X25" s="3">
+        <v>309.76748549322929</v>
+      </c>
+    </row>
+    <row r="26" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1380,8 +2617,18 @@
       <c r="T26" s="3">
         <v>273.79771760154659</v>
       </c>
-    </row>
-    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V26" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="W26" s="3">
+        <v>105.51011006289281</v>
+      </c>
+      <c r="X26" s="3">
+        <v>276.97215667311337</v>
+      </c>
+    </row>
+    <row r="27" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1422,8 +2669,18 @@
       <c r="T27" s="3">
         <v>257.77653288201083</v>
       </c>
-    </row>
-    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V27" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="W27" s="3">
+        <v>104.1006071601352</v>
+      </c>
+      <c r="X27" s="3">
+        <v>287.20216150870323</v>
+      </c>
+    </row>
+    <row r="28" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1464,8 +2721,18 @@
       <c r="T28" s="3">
         <v>284.24172630560838</v>
       </c>
-    </row>
-    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V28" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="W28" s="3">
+        <v>103.35170657958361</v>
+      </c>
+      <c r="X28" s="3">
+        <v>257.86702611218487</v>
+      </c>
+    </row>
+    <row r="29" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1506,8 +2773,18 @@
       <c r="T29" s="3">
         <v>265.30017408123717</v>
       </c>
-    </row>
-    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V29" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="W29" s="3">
+        <v>99.562106918238683</v>
+      </c>
+      <c r="X29" s="3">
+        <v>330.93872823984452</v>
+      </c>
+    </row>
+    <row r="30" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1548,8 +2825,18 @@
       <c r="T30" s="3">
         <v>277.44027562862601</v>
       </c>
-    </row>
-    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V30" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="W30" s="3">
+        <v>107.1463316400578</v>
+      </c>
+      <c r="X30" s="3">
+        <v>248.44185686653691</v>
+      </c>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1590,8 +2877,18 @@
       <c r="T31" s="3">
         <v>281.64653771760072</v>
       </c>
-    </row>
-    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V31" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="W31" s="3">
+        <v>103.5655696661826</v>
+      </c>
+      <c r="X31" s="3">
+        <v>298.76499999999919</v>
+      </c>
+    </row>
+    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1632,8 +2929,18 @@
       <c r="T32" s="3">
         <v>268.56069148936092</v>
       </c>
-    </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V32" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="W32" s="3">
+        <v>104.1855660377355</v>
+      </c>
+      <c r="X32" s="3">
+        <v>282.80219535783277</v>
+      </c>
+    </row>
+    <row r="33" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1674,8 +2981,18 @@
       <c r="T33" s="3">
         <v>293.82440038684638</v>
       </c>
-    </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V33" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="W33" s="3">
+        <v>104.9074806482823</v>
+      </c>
+      <c r="X33" s="3">
+        <v>263.84682785299731</v>
+      </c>
+    </row>
+    <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1716,8 +3033,18 @@
       <c r="T34" s="3">
         <v>262.06911025145001</v>
       </c>
-    </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V34" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="W34" s="3">
+        <v>104.3870936139329</v>
+      </c>
+      <c r="X34" s="3">
+        <v>262.04008220502823</v>
+      </c>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1758,8 +3085,18 @@
       <c r="T35" s="3">
         <v>277.19192456479612</v>
       </c>
-    </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V35" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="W35" s="3">
+        <v>104.64099177551979</v>
+      </c>
+      <c r="X35" s="3">
+        <v>269.91053191489277</v>
+      </c>
+    </row>
+    <row r="36" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1800,8 +3137,18 @@
       <c r="T36" s="3">
         <v>267.77281914893541</v>
       </c>
-    </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V36" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="W36" s="3">
+        <v>103.8842670537007</v>
+      </c>
+      <c r="X36" s="3">
+        <v>265.96865570599527</v>
+      </c>
+    </row>
+    <row r="37" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1842,8 +3189,18 @@
       <c r="T37" s="3">
         <v>282.78385880077292</v>
       </c>
-    </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V37" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="W37" s="3">
+        <v>103.5382111756165</v>
+      </c>
+      <c r="X37" s="3">
+        <v>270.53409574467997</v>
+      </c>
+    </row>
+    <row r="38" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1884,8 +3241,18 @@
       <c r="T38" s="3">
         <v>258.77467601547312</v>
       </c>
-    </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V38" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="W38" s="3">
+        <v>102.07266690856279</v>
+      </c>
+      <c r="X38" s="3">
+        <v>315.19343326885792</v>
+      </c>
+    </row>
+    <row r="39" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1926,8 +3293,18 @@
       <c r="T39" s="3">
         <v>274.68762572533763</v>
       </c>
-    </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V39" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="W39" s="3">
+        <v>104.57978108369591</v>
+      </c>
+      <c r="X39" s="3">
+        <v>268.67074468085019</v>
+      </c>
+    </row>
+    <row r="40" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1968,8 +3345,18 @@
       <c r="T40" s="3">
         <v>267.41830270792963</v>
       </c>
-    </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V40" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="W40" s="3">
+        <v>105.58822327044</v>
+      </c>
+      <c r="X40" s="3">
+        <v>258.25176982591802</v>
+      </c>
+    </row>
+    <row r="41" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2010,8 +3397,18 @@
       <c r="T41" s="3">
         <v>298.6525483558986</v>
       </c>
-    </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V41" s="2">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="W41" s="3">
+        <v>103.8068384131589</v>
+      </c>
+      <c r="X41" s="3">
+        <v>290.93927949709769</v>
+      </c>
+    </row>
+    <row r="42" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2052,8 +3449,18 @@
       <c r="T42" s="3">
         <v>263.5406673114112</v>
       </c>
-    </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V42" s="2">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="W42" s="3">
+        <v>103.2951100628928</v>
+      </c>
+      <c r="X42" s="3">
+        <v>290.70367504835508</v>
+      </c>
+    </row>
+    <row r="43" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2094,8 +3501,18 @@
       <c r="T43" s="3">
         <v>268.06646034816168</v>
       </c>
-    </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V43" s="2">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="W43" s="3">
+        <v>103.4801717464922</v>
+      </c>
+      <c r="X43" s="3">
+        <v>268.04074468085031</v>
+      </c>
+    </row>
+    <row r="44" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2136,8 +3553,18 @@
       <c r="T44" s="3">
         <v>273.42770309477669</v>
       </c>
-    </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V44" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="W44" s="3">
+        <v>106.2967767295595</v>
+      </c>
+      <c r="X44" s="3">
+        <v>255.37573500967039</v>
+      </c>
+    </row>
+    <row r="45" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2178,8 +3605,18 @@
       <c r="T45" s="3">
         <v>279.27834139264922</v>
       </c>
-    </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V45" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="W45" s="3">
+        <v>102.682890662796</v>
+      </c>
+      <c r="X45" s="3">
+        <v>292.17954545454472</v>
+      </c>
+    </row>
+    <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2220,8 +3657,18 @@
       <c r="T46" s="3">
         <v>278.94244680850989</v>
       </c>
-    </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V46" s="2">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="W46" s="3">
+        <v>102.63612360909499</v>
+      </c>
+      <c r="X46" s="3">
+        <v>310.36363636363558</v>
+      </c>
+    </row>
+    <row r="47" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2262,8 +3709,18 @@
       <c r="T47" s="3">
         <v>270.91570116054078</v>
       </c>
-    </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V47" s="2">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="W47" s="3">
+        <v>103.54432027092371</v>
+      </c>
+      <c r="X47" s="3">
+        <v>301.20269825918677</v>
+      </c>
+    </row>
+    <row r="48" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2304,8 +3761,18 @@
       <c r="T48" s="3">
         <v>272.83668278529899</v>
       </c>
-    </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V48" s="2">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="W48" s="3">
+        <v>102.2652733430089</v>
+      </c>
+      <c r="X48" s="3">
+        <v>297.47021760154649</v>
+      </c>
+    </row>
+    <row r="49" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2346,8 +3813,18 @@
       <c r="T49" s="3">
         <v>282.99298839458328</v>
       </c>
-    </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V49" s="2">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="W49" s="3">
+        <v>105.0254559748425</v>
+      </c>
+      <c r="X49" s="3">
+        <v>260.63614119922562</v>
+      </c>
+    </row>
+    <row r="50" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2388,8 +3865,18 @@
       <c r="T50" s="3">
         <v>258.98455512572451</v>
       </c>
-    </row>
-    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V50" s="2">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="W50" s="3">
+        <v>103.10429729075921</v>
+      </c>
+      <c r="X50" s="3">
+        <v>289.16570116054078</v>
+      </c>
+    </row>
+    <row r="51" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2430,8 +3917,18 @@
       <c r="T51" s="3">
         <v>272.8359574468077</v>
       </c>
-    </row>
-    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V51" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="W51" s="3">
+        <v>103.0661115142716</v>
+      </c>
+      <c r="X51" s="3">
+        <v>281.08353481624681</v>
+      </c>
+    </row>
+    <row r="52" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2472,8 +3969,18 @@
       <c r="T52" s="3">
         <v>285.45289651837442</v>
       </c>
-    </row>
-    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V52" s="2">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="W52" s="3">
+        <v>105.9801560232218</v>
+      </c>
+      <c r="X52" s="3">
+        <v>257.51771760154668</v>
+      </c>
+    </row>
+    <row r="53" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2514,8 +4021,18 @@
       <c r="T53" s="3">
         <v>259.88518858800688</v>
       </c>
-    </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V53" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="W53" s="3">
+        <v>104.26997097242349</v>
+      </c>
+      <c r="X53" s="3">
+        <v>273.44353965183672</v>
+      </c>
+    </row>
+    <row r="54" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2556,8 +4073,18 @@
       <c r="T54" s="3">
         <v>254.84565280464139</v>
       </c>
-    </row>
-    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V54" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="W54" s="3">
+        <v>103.4525991775517</v>
+      </c>
+      <c r="X54" s="3">
+        <v>283.08345261121792</v>
+      </c>
+    </row>
+    <row r="56" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2602,8 +4129,19 @@
         <f>AVERAGE(T5:T54)</f>
         <v>274.36524332688504</v>
       </c>
-    </row>
-    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="V56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W56" s="3">
+        <f>AVERAGE(W5:W54)</f>
+        <v>103.84828248669541</v>
+      </c>
+      <c r="X56" s="3">
+        <f>AVERAGE(X5:X54)</f>
+        <v>281.43923549322938</v>
+      </c>
+    </row>
+    <row r="57" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -2648,9 +4186,52 @@
         <f>_xlfn.STDEV.S(T5:T54)</f>
         <v>12.554493545564942</v>
       </c>
+      <c r="V57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W57" s="3">
+        <f>_xlfn.STDEV.S(W5:W54)</f>
+        <v>1.5781456866034163</v>
+      </c>
+      <c r="X57" s="3">
+        <f>_xlfn.STDEV.S(X5:X54)</f>
+        <v>21.613720633399581</v>
+      </c>
+    </row>
+    <row r="62" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="F62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="E63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="3">
+        <v>114.07751352160854</v>
+      </c>
+      <c r="G63" s="3">
+        <v>102.39860418480858</v>
+      </c>
+    </row>
+    <row r="64" spans="3:24" x14ac:dyDescent="0.25">
+      <c r="E64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="3">
+        <v>303.82919657827125</v>
+      </c>
+      <c r="G64" s="3">
+        <v>274.36524332688504</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2658,7 +4239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>

</xml_diff>